<commit_message>
Added actual units for time
</commit_message>
<xml_diff>
--- a/results/results_drug_on_mutation_of_Ras.xlsx
+++ b/results/results_drug_on_mutation_of_Ras.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4220" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4642" uniqueCount="422">
   <si>
     <t>Protein</t>
   </si>
@@ -1301,7 +1301,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1329,11 +1329,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1355,6 +1357,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1373,18 +1377,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19" t="s">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>420</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="21" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -1395,7 +1399,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -1406,7 +1410,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -1417,7 +1421,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="21" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -1428,7 +1432,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -1439,7 +1443,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -1450,7 +1454,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -1461,7 +1465,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -1472,7 +1476,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="21" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -1483,7 +1487,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -1494,7 +1498,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="21" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -1505,7 +1509,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -1516,7 +1520,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="21" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -1527,7 +1531,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -1538,7 +1542,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="21" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -1549,7 +1553,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="21" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -1560,7 +1564,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -1571,7 +1575,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -1582,7 +1586,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B20">
@@ -1593,7 +1597,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B21">
@@ -1604,7 +1608,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="21" t="s">
         <v>21</v>
       </c>
       <c r="B22">
@@ -1615,7 +1619,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B23">
@@ -1626,7 +1630,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B24">
@@ -1637,7 +1641,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="21" t="s">
         <v>24</v>
       </c>
       <c r="B25">
@@ -1648,7 +1652,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B26">
@@ -1659,7 +1663,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B27">
@@ -1670,7 +1674,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B28">
@@ -1681,7 +1685,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="21" t="s">
         <v>28</v>
       </c>
       <c r="B29">
@@ -1692,7 +1696,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="21" t="s">
         <v>29</v>
       </c>
       <c r="B30">
@@ -1703,7 +1707,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="21" t="s">
         <v>30</v>
       </c>
       <c r="B31">
@@ -1714,7 +1718,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="21" t="s">
         <v>31</v>
       </c>
       <c r="B32">
@@ -1725,7 +1729,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="21" t="s">
         <v>32</v>
       </c>
       <c r="B33">
@@ -1736,7 +1740,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B34">
@@ -1747,7 +1751,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="21" t="s">
         <v>34</v>
       </c>
       <c r="B35">
@@ -1758,7 +1762,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="21" t="s">
         <v>35</v>
       </c>
       <c r="B36">
@@ -1769,7 +1773,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B37">
@@ -1780,7 +1784,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B38">
@@ -1791,7 +1795,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="21" t="s">
         <v>38</v>
       </c>
       <c r="B39">
@@ -1802,7 +1806,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B40">
@@ -1813,7 +1817,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="21" t="s">
         <v>40</v>
       </c>
       <c r="B41">
@@ -1824,7 +1828,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B42">
@@ -1835,7 +1839,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B43">
@@ -1846,7 +1850,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B44">
@@ -1857,7 +1861,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="21" t="s">
         <v>44</v>
       </c>
       <c r="B45">
@@ -1868,7 +1872,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="21" t="s">
         <v>45</v>
       </c>
       <c r="B46">
@@ -1879,7 +1883,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="21" t="s">
         <v>46</v>
       </c>
       <c r="B47">
@@ -1890,7 +1894,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B48">
@@ -1901,7 +1905,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="21" t="s">
         <v>48</v>
       </c>
       <c r="B49">
@@ -1912,7 +1916,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B50">
@@ -1923,7 +1927,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="21" t="s">
         <v>50</v>
       </c>
       <c r="B51">
@@ -1934,7 +1938,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="21" t="s">
         <v>51</v>
       </c>
       <c r="B52">
@@ -1945,7 +1949,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="21" t="s">
         <v>52</v>
       </c>
       <c r="B53">
@@ -1956,7 +1960,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="19" t="s">
+      <c r="A54" s="21" t="s">
         <v>53</v>
       </c>
       <c r="B54">
@@ -1967,7 +1971,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="21" t="s">
         <v>54</v>
       </c>
       <c r="B55">
@@ -1978,7 +1982,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="19" t="s">
+      <c r="A56" s="21" t="s">
         <v>55</v>
       </c>
       <c r="B56">
@@ -1989,7 +1993,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="21" t="s">
         <v>56</v>
       </c>
       <c r="B57">
@@ -2000,7 +2004,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="19" t="s">
+      <c r="A58" s="21" t="s">
         <v>57</v>
       </c>
       <c r="B58">
@@ -2011,7 +2015,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="21" t="s">
         <v>58</v>
       </c>
       <c r="B59">
@@ -2022,7 +2026,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="19" t="s">
+      <c r="A60" s="21" t="s">
         <v>59</v>
       </c>
       <c r="B60">
@@ -2033,7 +2037,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="21" t="s">
         <v>60</v>
       </c>
       <c r="B61">
@@ -2044,7 +2048,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="19" t="s">
+      <c r="A62" s="21" t="s">
         <v>61</v>
       </c>
       <c r="B62">
@@ -2055,7 +2059,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="19" t="s">
+      <c r="A63" s="21" t="s">
         <v>62</v>
       </c>
       <c r="B63">
@@ -2066,7 +2070,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="19" t="s">
+      <c r="A64" s="21" t="s">
         <v>63</v>
       </c>
       <c r="B64">
@@ -2077,7 +2081,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="19" t="s">
+      <c r="A65" s="21" t="s">
         <v>64</v>
       </c>
       <c r="B65">
@@ -2088,7 +2092,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="21" t="s">
         <v>65</v>
       </c>
       <c r="B66">
@@ -2099,7 +2103,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="21" t="s">
         <v>66</v>
       </c>
       <c r="B67">
@@ -2110,7 +2114,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="19" t="s">
+      <c r="A68" s="21" t="s">
         <v>67</v>
       </c>
       <c r="B68">
@@ -2121,7 +2125,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="19" t="s">
+      <c r="A69" s="21" t="s">
         <v>68</v>
       </c>
       <c r="B69">
@@ -2132,7 +2136,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="19" t="s">
+      <c r="A70" s="21" t="s">
         <v>69</v>
       </c>
       <c r="B70">
@@ -2143,7 +2147,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="19" t="s">
+      <c r="A71" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B71">
@@ -2154,7 +2158,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="21" t="s">
         <v>71</v>
       </c>
       <c r="B72">
@@ -2165,7 +2169,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="19" t="s">
+      <c r="A73" s="21" t="s">
         <v>72</v>
       </c>
       <c r="B73">
@@ -2176,7 +2180,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="19" t="s">
+      <c r="A74" s="21" t="s">
         <v>73</v>
       </c>
       <c r="B74">
@@ -2187,7 +2191,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="19" t="s">
+      <c r="A75" s="21" t="s">
         <v>74</v>
       </c>
       <c r="B75">
@@ -2198,7 +2202,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="19" t="s">
+      <c r="A76" s="21" t="s">
         <v>75</v>
       </c>
       <c r="B76">
@@ -2209,7 +2213,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="19" t="s">
+      <c r="A77" s="21" t="s">
         <v>76</v>
       </c>
       <c r="B77">
@@ -2220,7 +2224,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="19" t="s">
+      <c r="A78" s="21" t="s">
         <v>77</v>
       </c>
       <c r="B78">
@@ -2231,7 +2235,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="21" t="s">
         <v>78</v>
       </c>
       <c r="B79">
@@ -2242,7 +2246,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="19" t="s">
+      <c r="A80" s="21" t="s">
         <v>79</v>
       </c>
       <c r="B80">
@@ -2253,7 +2257,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="19" t="s">
+      <c r="A81" s="21" t="s">
         <v>80</v>
       </c>
       <c r="B81">
@@ -2264,7 +2268,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="19" t="s">
+      <c r="A82" s="21" t="s">
         <v>81</v>
       </c>
       <c r="B82">
@@ -2275,7 +2279,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="19" t="s">
+      <c r="A83" s="21" t="s">
         <v>82</v>
       </c>
       <c r="B83">
@@ -2286,7 +2290,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="19" t="s">
+      <c r="A84" s="21" t="s">
         <v>83</v>
       </c>
       <c r="B84">
@@ -2297,7 +2301,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="19" t="s">
+      <c r="A85" s="21" t="s">
         <v>84</v>
       </c>
       <c r="B85">
@@ -2308,7 +2312,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="19" t="s">
+      <c r="A86" s="21" t="s">
         <v>85</v>
       </c>
       <c r="B86">
@@ -2319,7 +2323,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="19" t="s">
+      <c r="A87" s="21" t="s">
         <v>86</v>
       </c>
       <c r="B87">
@@ -2330,7 +2334,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="19" t="s">
+      <c r="A88" s="21" t="s">
         <v>87</v>
       </c>
       <c r="B88">
@@ -2341,7 +2345,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="19" t="s">
+      <c r="A89" s="21" t="s">
         <v>88</v>
       </c>
       <c r="B89">
@@ -2352,7 +2356,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="19" t="s">
+      <c r="A90" s="21" t="s">
         <v>89</v>
       </c>
       <c r="B90">
@@ -2363,7 +2367,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="19" t="s">
+      <c r="A91" s="21" t="s">
         <v>90</v>
       </c>
       <c r="B91">
@@ -2374,7 +2378,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="19" t="s">
+      <c r="A92" s="21" t="s">
         <v>91</v>
       </c>
       <c r="B92">
@@ -2385,7 +2389,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="19" t="s">
+      <c r="A93" s="21" t="s">
         <v>92</v>
       </c>
       <c r="B93">
@@ -2396,7 +2400,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="19" t="s">
+      <c r="A94" s="21" t="s">
         <v>93</v>
       </c>
       <c r="B94">
@@ -2407,7 +2411,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="19" t="s">
+      <c r="A95" s="21" t="s">
         <v>94</v>
       </c>
       <c r="B95">
@@ -2418,7 +2422,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="19" t="s">
+      <c r="A96" s="21" t="s">
         <v>95</v>
       </c>
       <c r="B96">
@@ -2429,7 +2433,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="19" t="s">
+      <c r="A97" s="21" t="s">
         <v>96</v>
       </c>
       <c r="B97">
@@ -2440,7 +2444,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="19" t="s">
+      <c r="A98" s="21" t="s">
         <v>97</v>
       </c>
       <c r="B98">
@@ -2451,7 +2455,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="19" t="s">
+      <c r="A99" s="21" t="s">
         <v>98</v>
       </c>
       <c r="B99">
@@ -2462,7 +2466,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="19" t="s">
+      <c r="A100" s="21" t="s">
         <v>99</v>
       </c>
       <c r="B100">
@@ -2473,7 +2477,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="21" t="s">
         <v>100</v>
       </c>
       <c r="B101">
@@ -2484,7 +2488,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="19" t="s">
+      <c r="A102" s="21" t="s">
         <v>101</v>
       </c>
       <c r="B102">
@@ -2495,7 +2499,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="19" t="s">
+      <c r="A103" s="21" t="s">
         <v>102</v>
       </c>
       <c r="B103">
@@ -2506,7 +2510,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="19" t="s">
+      <c r="A104" s="21" t="s">
         <v>103</v>
       </c>
       <c r="B104">
@@ -2517,7 +2521,7 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="19" t="s">
+      <c r="A105" s="21" t="s">
         <v>104</v>
       </c>
       <c r="B105">
@@ -2528,7 +2532,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="19" t="s">
+      <c r="A106" s="21" t="s">
         <v>105</v>
       </c>
       <c r="B106">
@@ -2539,7 +2543,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="19" t="s">
+      <c r="A107" s="21" t="s">
         <v>106</v>
       </c>
       <c r="B107">
@@ -2550,7 +2554,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="19" t="s">
+      <c r="A108" s="21" t="s">
         <v>107</v>
       </c>
       <c r="B108">
@@ -2561,7 +2565,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="19" t="s">
+      <c r="A109" s="21" t="s">
         <v>108</v>
       </c>
       <c r="B109">
@@ -2572,7 +2576,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="19" t="s">
+      <c r="A110" s="21" t="s">
         <v>109</v>
       </c>
       <c r="B110">
@@ -2583,7 +2587,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="19" t="s">
+      <c r="A111" s="21" t="s">
         <v>110</v>
       </c>
       <c r="B111">
@@ -2594,7 +2598,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="19" t="s">
+      <c r="A112" s="21" t="s">
         <v>111</v>
       </c>
       <c r="B112">
@@ -2605,7 +2609,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="19" t="s">
+      <c r="A113" s="21" t="s">
         <v>112</v>
       </c>
       <c r="B113">
@@ -2616,7 +2620,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="19" t="s">
+      <c r="A114" s="21" t="s">
         <v>113</v>
       </c>
       <c r="B114">
@@ -2627,7 +2631,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="19" t="s">
+      <c r="A115" s="21" t="s">
         <v>114</v>
       </c>
       <c r="B115">
@@ -2638,7 +2642,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="19" t="s">
+      <c r="A116" s="21" t="s">
         <v>115</v>
       </c>
       <c r="B116">
@@ -2649,7 +2653,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="19" t="s">
+      <c r="A117" s="21" t="s">
         <v>116</v>
       </c>
       <c r="B117">
@@ -2660,7 +2664,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="19" t="s">
+      <c r="A118" s="21" t="s">
         <v>117</v>
       </c>
       <c r="B118">
@@ -2671,7 +2675,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="19" t="s">
+      <c r="A119" s="21" t="s">
         <v>118</v>
       </c>
       <c r="B119">
@@ -2682,7 +2686,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="19" t="s">
+      <c r="A120" s="21" t="s">
         <v>119</v>
       </c>
       <c r="B120">
@@ -2693,7 +2697,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="19" t="s">
+      <c r="A121" s="21" t="s">
         <v>120</v>
       </c>
       <c r="B121">
@@ -2704,7 +2708,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="19" t="s">
+      <c r="A122" s="21" t="s">
         <v>121</v>
       </c>
       <c r="B122">
@@ -2715,7 +2719,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="19" t="s">
+      <c r="A123" s="21" t="s">
         <v>122</v>
       </c>
       <c r="B123">
@@ -2726,7 +2730,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="19" t="s">
+      <c r="A124" s="21" t="s">
         <v>123</v>
       </c>
       <c r="B124">
@@ -2737,7 +2741,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="19" t="s">
+      <c r="A125" s="21" t="s">
         <v>124</v>
       </c>
       <c r="B125">
@@ -2748,7 +2752,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="19" t="s">
+      <c r="A126" s="21" t="s">
         <v>125</v>
       </c>
       <c r="B126">
@@ -2759,7 +2763,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="19" t="s">
+      <c r="A127" s="21" t="s">
         <v>126</v>
       </c>
       <c r="B127">
@@ -2770,7 +2774,7 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="19" t="s">
+      <c r="A128" s="21" t="s">
         <v>127</v>
       </c>
       <c r="B128">
@@ -2781,7 +2785,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="19" t="s">
+      <c r="A129" s="21" t="s">
         <v>128</v>
       </c>
       <c r="B129">
@@ -2792,7 +2796,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="19" t="s">
+      <c r="A130" s="21" t="s">
         <v>129</v>
       </c>
       <c r="B130">
@@ -2803,7 +2807,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="19" t="s">
+      <c r="A131" s="21" t="s">
         <v>130</v>
       </c>
       <c r="B131">
@@ -2814,7 +2818,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="19" t="s">
+      <c r="A132" s="21" t="s">
         <v>131</v>
       </c>
       <c r="B132">
@@ -2825,7 +2829,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="19" t="s">
+      <c r="A133" s="21" t="s">
         <v>132</v>
       </c>
       <c r="B133">
@@ -2836,7 +2840,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="19" t="s">
+      <c r="A134" s="21" t="s">
         <v>133</v>
       </c>
       <c r="B134">
@@ -2847,7 +2851,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="19" t="s">
+      <c r="A135" s="21" t="s">
         <v>134</v>
       </c>
       <c r="B135">
@@ -2858,7 +2862,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="19" t="s">
+      <c r="A136" s="21" t="s">
         <v>135</v>
       </c>
       <c r="B136">
@@ -2869,7 +2873,7 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="19" t="s">
+      <c r="A137" s="21" t="s">
         <v>136</v>
       </c>
       <c r="B137">
@@ -2880,7 +2884,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="19" t="s">
+      <c r="A138" s="21" t="s">
         <v>137</v>
       </c>
       <c r="B138">
@@ -2891,7 +2895,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="19" t="s">
+      <c r="A139" s="21" t="s">
         <v>138</v>
       </c>
       <c r="B139">
@@ -2902,7 +2906,7 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="19" t="s">
+      <c r="A140" s="21" t="s">
         <v>139</v>
       </c>
       <c r="B140">
@@ -2913,7 +2917,7 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="19" t="s">
+      <c r="A141" s="21" t="s">
         <v>140</v>
       </c>
       <c r="B141">
@@ -2924,7 +2928,7 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="19" t="s">
+      <c r="A142" s="21" t="s">
         <v>141</v>
       </c>
       <c r="B142">
@@ -2935,7 +2939,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="19" t="s">
+      <c r="A143" s="21" t="s">
         <v>142</v>
       </c>
       <c r="B143">
@@ -2946,7 +2950,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="19" t="s">
+      <c r="A144" s="21" t="s">
         <v>143</v>
       </c>
       <c r="B144">
@@ -2957,7 +2961,7 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="19" t="s">
+      <c r="A145" s="21" t="s">
         <v>144</v>
       </c>
       <c r="B145">
@@ -2968,7 +2972,7 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="19" t="s">
+      <c r="A146" s="21" t="s">
         <v>145</v>
       </c>
       <c r="B146">
@@ -2979,7 +2983,7 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="19" t="s">
+      <c r="A147" s="21" t="s">
         <v>146</v>
       </c>
       <c r="B147">
@@ -2990,7 +2994,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="19" t="s">
+      <c r="A148" s="21" t="s">
         <v>147</v>
       </c>
       <c r="B148">
@@ -3001,7 +3005,7 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="19" t="s">
+      <c r="A149" s="21" t="s">
         <v>148</v>
       </c>
       <c r="B149">
@@ -3012,7 +3016,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="19" t="s">
+      <c r="A150" s="21" t="s">
         <v>149</v>
       </c>
       <c r="B150">
@@ -3023,7 +3027,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="19" t="s">
+      <c r="A151" s="21" t="s">
         <v>150</v>
       </c>
       <c r="B151">
@@ -3034,7 +3038,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="19" t="s">
+      <c r="A152" s="21" t="s">
         <v>151</v>
       </c>
       <c r="B152">
@@ -3045,7 +3049,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="19" t="s">
+      <c r="A153" s="21" t="s">
         <v>152</v>
       </c>
       <c r="B153">
@@ -3056,7 +3060,7 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="19" t="s">
+      <c r="A154" s="21" t="s">
         <v>153</v>
       </c>
       <c r="B154">
@@ -3067,7 +3071,7 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="19" t="s">
+      <c r="A155" s="21" t="s">
         <v>154</v>
       </c>
       <c r="B155">
@@ -3078,7 +3082,7 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="19" t="s">
+      <c r="A156" s="21" t="s">
         <v>155</v>
       </c>
       <c r="B156">
@@ -3089,7 +3093,7 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="19" t="s">
+      <c r="A157" s="21" t="s">
         <v>156</v>
       </c>
       <c r="B157">
@@ -3100,7 +3104,7 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="19" t="s">
+      <c r="A158" s="21" t="s">
         <v>157</v>
       </c>
       <c r="B158">
@@ -3111,7 +3115,7 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="19" t="s">
+      <c r="A159" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B159">
@@ -3122,7 +3126,7 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="19" t="s">
+      <c r="A160" s="21" t="s">
         <v>159</v>
       </c>
       <c r="B160">
@@ -3133,7 +3137,7 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="19" t="s">
+      <c r="A161" s="21" t="s">
         <v>160</v>
       </c>
       <c r="B161">
@@ -3144,7 +3148,7 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="19" t="s">
+      <c r="A162" s="21" t="s">
         <v>161</v>
       </c>
       <c r="B162">
@@ -3155,7 +3159,7 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="19" t="s">
+      <c r="A163" s="21" t="s">
         <v>162</v>
       </c>
       <c r="B163">
@@ -3166,7 +3170,7 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="19" t="s">
+      <c r="A164" s="21" t="s">
         <v>163</v>
       </c>
       <c r="B164">
@@ -3177,7 +3181,7 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="19" t="s">
+      <c r="A165" s="21" t="s">
         <v>164</v>
       </c>
       <c r="B165">
@@ -3188,7 +3192,7 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" s="19" t="s">
+      <c r="A166" s="21" t="s">
         <v>165</v>
       </c>
       <c r="B166">
@@ -3199,7 +3203,7 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="19" t="s">
+      <c r="A167" s="21" t="s">
         <v>166</v>
       </c>
       <c r="B167">
@@ -3210,7 +3214,7 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="19" t="s">
+      <c r="A168" s="21" t="s">
         <v>167</v>
       </c>
       <c r="B168">
@@ -3221,7 +3225,7 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="19" t="s">
+      <c r="A169" s="21" t="s">
         <v>168</v>
       </c>
       <c r="B169">
@@ -3232,7 +3236,7 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="19" t="s">
+      <c r="A170" s="21" t="s">
         <v>169</v>
       </c>
       <c r="B170">
@@ -3243,7 +3247,7 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="19" t="s">
+      <c r="A171" s="21" t="s">
         <v>170</v>
       </c>
       <c r="B171">
@@ -3254,7 +3258,7 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="19" t="s">
+      <c r="A172" s="21" t="s">
         <v>171</v>
       </c>
       <c r="B172">
@@ -3265,7 +3269,7 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="19" t="s">
+      <c r="A173" s="21" t="s">
         <v>172</v>
       </c>
       <c r="B173">
@@ -3276,7 +3280,7 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="19" t="s">
+      <c r="A174" s="21" t="s">
         <v>173</v>
       </c>
       <c r="B174">
@@ -3287,7 +3291,7 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" s="19" t="s">
+      <c r="A175" s="21" t="s">
         <v>174</v>
       </c>
       <c r="B175">
@@ -3298,7 +3302,7 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="19" t="s">
+      <c r="A176" s="21" t="s">
         <v>175</v>
       </c>
       <c r="B176">
@@ -3309,7 +3313,7 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="19" t="s">
+      <c r="A177" s="21" t="s">
         <v>176</v>
       </c>
       <c r="B177">
@@ -3320,7 +3324,7 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="19" t="s">
+      <c r="A178" s="21" t="s">
         <v>177</v>
       </c>
       <c r="B178">
@@ -3331,7 +3335,7 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" s="19" t="s">
+      <c r="A179" s="21" t="s">
         <v>178</v>
       </c>
       <c r="B179">
@@ -3342,7 +3346,7 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="19" t="s">
+      <c r="A180" s="21" t="s">
         <v>179</v>
       </c>
       <c r="B180">
@@ -3353,7 +3357,7 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" s="19" t="s">
+      <c r="A181" s="21" t="s">
         <v>180</v>
       </c>
       <c r="B181">
@@ -3364,7 +3368,7 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" s="19" t="s">
+      <c r="A182" s="21" t="s">
         <v>181</v>
       </c>
       <c r="B182">
@@ -3375,7 +3379,7 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" s="19" t="s">
+      <c r="A183" s="21" t="s">
         <v>182</v>
       </c>
       <c r="B183">
@@ -3386,7 +3390,7 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="19" t="s">
+      <c r="A184" s="21" t="s">
         <v>183</v>
       </c>
       <c r="B184">
@@ -3397,7 +3401,7 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" s="19" t="s">
+      <c r="A185" s="21" t="s">
         <v>184</v>
       </c>
       <c r="B185">
@@ -3408,7 +3412,7 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" s="19" t="s">
+      <c r="A186" s="21" t="s">
         <v>185</v>
       </c>
       <c r="B186">
@@ -3419,7 +3423,7 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" s="19" t="s">
+      <c r="A187" s="21" t="s">
         <v>186</v>
       </c>
       <c r="B187">
@@ -3430,7 +3434,7 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" s="19" t="s">
+      <c r="A188" s="21" t="s">
         <v>187</v>
       </c>
       <c r="B188">
@@ -3441,7 +3445,7 @@
       </c>
     </row>
     <row r="189">
-      <c r="A189" s="19" t="s">
+      <c r="A189" s="21" t="s">
         <v>188</v>
       </c>
       <c r="B189">
@@ -3452,7 +3456,7 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" s="19" t="s">
+      <c r="A190" s="21" t="s">
         <v>189</v>
       </c>
       <c r="B190">
@@ -3463,7 +3467,7 @@
       </c>
     </row>
     <row r="191">
-      <c r="A191" s="19" t="s">
+      <c r="A191" s="21" t="s">
         <v>190</v>
       </c>
       <c r="B191">
@@ -3474,7 +3478,7 @@
       </c>
     </row>
     <row r="192">
-      <c r="A192" s="19" t="s">
+      <c r="A192" s="21" t="s">
         <v>191</v>
       </c>
       <c r="B192">
@@ -3485,7 +3489,7 @@
       </c>
     </row>
     <row r="193">
-      <c r="A193" s="19" t="s">
+      <c r="A193" s="21" t="s">
         <v>192</v>
       </c>
       <c r="B193">
@@ -3496,7 +3500,7 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" s="19" t="s">
+      <c r="A194" s="21" t="s">
         <v>193</v>
       </c>
       <c r="B194">
@@ -3507,7 +3511,7 @@
       </c>
     </row>
     <row r="195">
-      <c r="A195" s="19" t="s">
+      <c r="A195" s="21" t="s">
         <v>194</v>
       </c>
       <c r="B195">
@@ -3518,7 +3522,7 @@
       </c>
     </row>
     <row r="196">
-      <c r="A196" s="19" t="s">
+      <c r="A196" s="21" t="s">
         <v>195</v>
       </c>
       <c r="B196">
@@ -3529,7 +3533,7 @@
       </c>
     </row>
     <row r="197">
-      <c r="A197" s="19" t="s">
+      <c r="A197" s="21" t="s">
         <v>196</v>
       </c>
       <c r="B197">
@@ -3540,7 +3544,7 @@
       </c>
     </row>
     <row r="198">
-      <c r="A198" s="19" t="s">
+      <c r="A198" s="21" t="s">
         <v>197</v>
       </c>
       <c r="B198">
@@ -3551,7 +3555,7 @@
       </c>
     </row>
     <row r="199">
-      <c r="A199" s="19" t="s">
+      <c r="A199" s="21" t="s">
         <v>198</v>
       </c>
       <c r="B199">
@@ -3562,7 +3566,7 @@
       </c>
     </row>
     <row r="200">
-      <c r="A200" s="19" t="s">
+      <c r="A200" s="21" t="s">
         <v>199</v>
       </c>
       <c r="B200">
@@ -3573,7 +3577,7 @@
       </c>
     </row>
     <row r="201">
-      <c r="A201" s="19" t="s">
+      <c r="A201" s="21" t="s">
         <v>200</v>
       </c>
       <c r="B201">
@@ -3584,7 +3588,7 @@
       </c>
     </row>
     <row r="202">
-      <c r="A202" s="19" t="s">
+      <c r="A202" s="21" t="s">
         <v>201</v>
       </c>
       <c r="B202">
@@ -3595,7 +3599,7 @@
       </c>
     </row>
     <row r="203">
-      <c r="A203" s="19" t="s">
+      <c r="A203" s="21" t="s">
         <v>202</v>
       </c>
       <c r="B203">
@@ -3606,7 +3610,7 @@
       </c>
     </row>
     <row r="204">
-      <c r="A204" s="19" t="s">
+      <c r="A204" s="21" t="s">
         <v>203</v>
       </c>
       <c r="B204">
@@ -3617,7 +3621,7 @@
       </c>
     </row>
     <row r="205">
-      <c r="A205" s="19" t="s">
+      <c r="A205" s="21" t="s">
         <v>204</v>
       </c>
       <c r="B205">
@@ -3628,7 +3632,7 @@
       </c>
     </row>
     <row r="206">
-      <c r="A206" s="19" t="s">
+      <c r="A206" s="21" t="s">
         <v>205</v>
       </c>
       <c r="B206">
@@ -3639,7 +3643,7 @@
       </c>
     </row>
     <row r="207">
-      <c r="A207" s="19" t="s">
+      <c r="A207" s="21" t="s">
         <v>206</v>
       </c>
       <c r="B207">
@@ -3650,7 +3654,7 @@
       </c>
     </row>
     <row r="208">
-      <c r="A208" s="19" t="s">
+      <c r="A208" s="21" t="s">
         <v>207</v>
       </c>
       <c r="B208">
@@ -3661,7 +3665,7 @@
       </c>
     </row>
     <row r="209">
-      <c r="A209" s="19" t="s">
+      <c r="A209" s="21" t="s">
         <v>208</v>
       </c>
       <c r="B209">
@@ -3672,7 +3676,7 @@
       </c>
     </row>
     <row r="210">
-      <c r="A210" s="19" t="s">
+      <c r="A210" s="21" t="s">
         <v>209</v>
       </c>
       <c r="B210">
@@ -3683,7 +3687,7 @@
       </c>
     </row>
     <row r="211">
-      <c r="A211" s="19" t="s">
+      <c r="A211" s="21" t="s">
         <v>210</v>
       </c>
       <c r="B211">
@@ -3694,7 +3698,7 @@
       </c>
     </row>
     <row r="212">
-      <c r="A212" s="19" t="s">
+      <c r="A212" s="21" t="s">
         <v>211</v>
       </c>
       <c r="B212">
@@ -3705,7 +3709,7 @@
       </c>
     </row>
     <row r="213">
-      <c r="A213" s="19" t="s">
+      <c r="A213" s="21" t="s">
         <v>212</v>
       </c>
       <c r="B213">
@@ -3716,7 +3720,7 @@
       </c>
     </row>
     <row r="214">
-      <c r="A214" s="19" t="s">
+      <c r="A214" s="21" t="s">
         <v>213</v>
       </c>
       <c r="B214">
@@ -3727,7 +3731,7 @@
       </c>
     </row>
     <row r="215">
-      <c r="A215" s="19" t="s">
+      <c r="A215" s="21" t="s">
         <v>214</v>
       </c>
       <c r="B215">
@@ -3738,7 +3742,7 @@
       </c>
     </row>
     <row r="216">
-      <c r="A216" s="19" t="s">
+      <c r="A216" s="21" t="s">
         <v>215</v>
       </c>
       <c r="B216">
@@ -3749,7 +3753,7 @@
       </c>
     </row>
     <row r="217">
-      <c r="A217" s="19" t="s">
+      <c r="A217" s="21" t="s">
         <v>216</v>
       </c>
       <c r="B217">
@@ -3760,7 +3764,7 @@
       </c>
     </row>
     <row r="218">
-      <c r="A218" s="19" t="s">
+      <c r="A218" s="21" t="s">
         <v>217</v>
       </c>
       <c r="B218">
@@ -3771,7 +3775,7 @@
       </c>
     </row>
     <row r="219">
-      <c r="A219" s="19" t="s">
+      <c r="A219" s="21" t="s">
         <v>218</v>
       </c>
       <c r="B219">
@@ -3782,7 +3786,7 @@
       </c>
     </row>
     <row r="220">
-      <c r="A220" s="19" t="s">
+      <c r="A220" s="21" t="s">
         <v>219</v>
       </c>
       <c r="B220">
@@ -3793,7 +3797,7 @@
       </c>
     </row>
     <row r="221">
-      <c r="A221" s="19" t="s">
+      <c r="A221" s="21" t="s">
         <v>220</v>
       </c>
       <c r="B221">
@@ -3804,7 +3808,7 @@
       </c>
     </row>
     <row r="222">
-      <c r="A222" s="19" t="s">
+      <c r="A222" s="21" t="s">
         <v>221</v>
       </c>
       <c r="B222">
@@ -3815,7 +3819,7 @@
       </c>
     </row>
     <row r="223">
-      <c r="A223" s="19" t="s">
+      <c r="A223" s="21" t="s">
         <v>222</v>
       </c>
       <c r="B223">
@@ -3826,7 +3830,7 @@
       </c>
     </row>
     <row r="224">
-      <c r="A224" s="19" t="s">
+      <c r="A224" s="21" t="s">
         <v>223</v>
       </c>
       <c r="B224">
@@ -3837,7 +3841,7 @@
       </c>
     </row>
     <row r="225">
-      <c r="A225" s="19" t="s">
+      <c r="A225" s="21" t="s">
         <v>224</v>
       </c>
       <c r="B225">
@@ -3848,7 +3852,7 @@
       </c>
     </row>
     <row r="226">
-      <c r="A226" s="19" t="s">
+      <c r="A226" s="21" t="s">
         <v>225</v>
       </c>
       <c r="B226">
@@ -3859,7 +3863,7 @@
       </c>
     </row>
     <row r="227">
-      <c r="A227" s="19" t="s">
+      <c r="A227" s="21" t="s">
         <v>226</v>
       </c>
       <c r="B227">
@@ -3870,7 +3874,7 @@
       </c>
     </row>
     <row r="228">
-      <c r="A228" s="19" t="s">
+      <c r="A228" s="21" t="s">
         <v>227</v>
       </c>
       <c r="B228">
@@ -3881,7 +3885,7 @@
       </c>
     </row>
     <row r="229">
-      <c r="A229" s="19" t="s">
+      <c r="A229" s="21" t="s">
         <v>228</v>
       </c>
       <c r="B229">
@@ -3892,7 +3896,7 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" s="19" t="s">
+      <c r="A230" s="21" t="s">
         <v>229</v>
       </c>
       <c r="B230">
@@ -3903,7 +3907,7 @@
       </c>
     </row>
     <row r="231">
-      <c r="A231" s="19" t="s">
+      <c r="A231" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B231">
@@ -3914,7 +3918,7 @@
       </c>
     </row>
     <row r="232">
-      <c r="A232" s="19" t="s">
+      <c r="A232" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B232">
@@ -3925,7 +3929,7 @@
       </c>
     </row>
     <row r="233">
-      <c r="A233" s="19" t="s">
+      <c r="A233" s="21" t="s">
         <v>232</v>
       </c>
       <c r="B233">
@@ -3936,7 +3940,7 @@
       </c>
     </row>
     <row r="234">
-      <c r="A234" s="19" t="s">
+      <c r="A234" s="21" t="s">
         <v>233</v>
       </c>
       <c r="B234">
@@ -3947,7 +3951,7 @@
       </c>
     </row>
     <row r="235">
-      <c r="A235" s="19" t="s">
+      <c r="A235" s="21" t="s">
         <v>234</v>
       </c>
       <c r="B235">
@@ -3958,7 +3962,7 @@
       </c>
     </row>
     <row r="236">
-      <c r="A236" s="19" t="s">
+      <c r="A236" s="21" t="s">
         <v>235</v>
       </c>
       <c r="B236">
@@ -3969,7 +3973,7 @@
       </c>
     </row>
     <row r="237">
-      <c r="A237" s="19" t="s">
+      <c r="A237" s="21" t="s">
         <v>236</v>
       </c>
       <c r="B237">
@@ -3980,7 +3984,7 @@
       </c>
     </row>
     <row r="238">
-      <c r="A238" s="19" t="s">
+      <c r="A238" s="21" t="s">
         <v>237</v>
       </c>
       <c r="B238">
@@ -3991,7 +3995,7 @@
       </c>
     </row>
     <row r="239">
-      <c r="A239" s="19" t="s">
+      <c r="A239" s="21" t="s">
         <v>238</v>
       </c>
       <c r="B239">
@@ -4002,7 +4006,7 @@
       </c>
     </row>
     <row r="240">
-      <c r="A240" s="19" t="s">
+      <c r="A240" s="21" t="s">
         <v>239</v>
       </c>
       <c r="B240">
@@ -4013,7 +4017,7 @@
       </c>
     </row>
     <row r="241">
-      <c r="A241" s="19" t="s">
+      <c r="A241" s="21" t="s">
         <v>240</v>
       </c>
       <c r="B241">
@@ -4024,7 +4028,7 @@
       </c>
     </row>
     <row r="242">
-      <c r="A242" s="19" t="s">
+      <c r="A242" s="21" t="s">
         <v>241</v>
       </c>
       <c r="B242">
@@ -4035,7 +4039,7 @@
       </c>
     </row>
     <row r="243">
-      <c r="A243" s="19" t="s">
+      <c r="A243" s="21" t="s">
         <v>242</v>
       </c>
       <c r="B243">
@@ -4046,7 +4050,7 @@
       </c>
     </row>
     <row r="244">
-      <c r="A244" s="19" t="s">
+      <c r="A244" s="21" t="s">
         <v>243</v>
       </c>
       <c r="B244">
@@ -4057,7 +4061,7 @@
       </c>
     </row>
     <row r="245">
-      <c r="A245" s="19" t="s">
+      <c r="A245" s="21" t="s">
         <v>244</v>
       </c>
       <c r="B245">
@@ -4068,7 +4072,7 @@
       </c>
     </row>
     <row r="246">
-      <c r="A246" s="19" t="s">
+      <c r="A246" s="21" t="s">
         <v>245</v>
       </c>
       <c r="B246">
@@ -4079,7 +4083,7 @@
       </c>
     </row>
     <row r="247">
-      <c r="A247" s="19" t="s">
+      <c r="A247" s="21" t="s">
         <v>246</v>
       </c>
       <c r="B247">
@@ -4090,7 +4094,7 @@
       </c>
     </row>
     <row r="248">
-      <c r="A248" s="19" t="s">
+      <c r="A248" s="21" t="s">
         <v>247</v>
       </c>
       <c r="B248">
@@ -4101,7 +4105,7 @@
       </c>
     </row>
     <row r="249">
-      <c r="A249" s="19" t="s">
+      <c r="A249" s="21" t="s">
         <v>248</v>
       </c>
       <c r="B249">
@@ -4112,7 +4116,7 @@
       </c>
     </row>
     <row r="250">
-      <c r="A250" s="19" t="s">
+      <c r="A250" s="21" t="s">
         <v>249</v>
       </c>
       <c r="B250">
@@ -4123,7 +4127,7 @@
       </c>
     </row>
     <row r="251">
-      <c r="A251" s="19" t="s">
+      <c r="A251" s="21" t="s">
         <v>250</v>
       </c>
       <c r="B251">
@@ -4134,7 +4138,7 @@
       </c>
     </row>
     <row r="252">
-      <c r="A252" s="19" t="s">
+      <c r="A252" s="21" t="s">
         <v>251</v>
       </c>
       <c r="B252">
@@ -4145,7 +4149,7 @@
       </c>
     </row>
     <row r="253">
-      <c r="A253" s="19" t="s">
+      <c r="A253" s="21" t="s">
         <v>252</v>
       </c>
       <c r="B253">
@@ -4156,7 +4160,7 @@
       </c>
     </row>
     <row r="254">
-      <c r="A254" s="19" t="s">
+      <c r="A254" s="21" t="s">
         <v>253</v>
       </c>
       <c r="B254">
@@ -4167,7 +4171,7 @@
       </c>
     </row>
     <row r="255">
-      <c r="A255" s="19" t="s">
+      <c r="A255" s="21" t="s">
         <v>254</v>
       </c>
       <c r="B255">
@@ -4178,7 +4182,7 @@
       </c>
     </row>
     <row r="256">
-      <c r="A256" s="19" t="s">
+      <c r="A256" s="21" t="s">
         <v>255</v>
       </c>
       <c r="B256">
@@ -4189,7 +4193,7 @@
       </c>
     </row>
     <row r="257">
-      <c r="A257" s="19" t="s">
+      <c r="A257" s="21" t="s">
         <v>256</v>
       </c>
       <c r="B257">
@@ -4200,7 +4204,7 @@
       </c>
     </row>
     <row r="258">
-      <c r="A258" s="19" t="s">
+      <c r="A258" s="21" t="s">
         <v>257</v>
       </c>
       <c r="B258">
@@ -4211,7 +4215,7 @@
       </c>
     </row>
     <row r="259">
-      <c r="A259" s="19" t="s">
+      <c r="A259" s="21" t="s">
         <v>258</v>
       </c>
       <c r="B259">
@@ -4222,7 +4226,7 @@
       </c>
     </row>
     <row r="260">
-      <c r="A260" s="19" t="s">
+      <c r="A260" s="21" t="s">
         <v>259</v>
       </c>
       <c r="B260">
@@ -4233,7 +4237,7 @@
       </c>
     </row>
     <row r="261">
-      <c r="A261" s="19" t="s">
+      <c r="A261" s="21" t="s">
         <v>260</v>
       </c>
       <c r="B261">
@@ -4244,7 +4248,7 @@
       </c>
     </row>
     <row r="262">
-      <c r="A262" s="19" t="s">
+      <c r="A262" s="21" t="s">
         <v>261</v>
       </c>
       <c r="B262">
@@ -4255,7 +4259,7 @@
       </c>
     </row>
     <row r="263">
-      <c r="A263" s="19" t="s">
+      <c r="A263" s="21" t="s">
         <v>262</v>
       </c>
       <c r="B263">
@@ -4266,7 +4270,7 @@
       </c>
     </row>
     <row r="264">
-      <c r="A264" s="19" t="s">
+      <c r="A264" s="21" t="s">
         <v>263</v>
       </c>
       <c r="B264">
@@ -4277,7 +4281,7 @@
       </c>
     </row>
     <row r="265">
-      <c r="A265" s="19" t="s">
+      <c r="A265" s="21" t="s">
         <v>264</v>
       </c>
       <c r="B265">
@@ -4288,7 +4292,7 @@
       </c>
     </row>
     <row r="266">
-      <c r="A266" s="19" t="s">
+      <c r="A266" s="21" t="s">
         <v>265</v>
       </c>
       <c r="B266">
@@ -4299,7 +4303,7 @@
       </c>
     </row>
     <row r="267">
-      <c r="A267" s="19" t="s">
+      <c r="A267" s="21" t="s">
         <v>266</v>
       </c>
       <c r="B267">
@@ -4310,7 +4314,7 @@
       </c>
     </row>
     <row r="268">
-      <c r="A268" s="19" t="s">
+      <c r="A268" s="21" t="s">
         <v>267</v>
       </c>
       <c r="B268">
@@ -4321,7 +4325,7 @@
       </c>
     </row>
     <row r="269">
-      <c r="A269" s="19" t="s">
+      <c r="A269" s="21" t="s">
         <v>268</v>
       </c>
       <c r="B269">
@@ -4332,7 +4336,7 @@
       </c>
     </row>
     <row r="270">
-      <c r="A270" s="19" t="s">
+      <c r="A270" s="21" t="s">
         <v>269</v>
       </c>
       <c r="B270">
@@ -4343,7 +4347,7 @@
       </c>
     </row>
     <row r="271">
-      <c r="A271" s="19" t="s">
+      <c r="A271" s="21" t="s">
         <v>270</v>
       </c>
       <c r="B271">
@@ -4354,7 +4358,7 @@
       </c>
     </row>
     <row r="272">
-      <c r="A272" s="19" t="s">
+      <c r="A272" s="21" t="s">
         <v>271</v>
       </c>
       <c r="B272">
@@ -4365,7 +4369,7 @@
       </c>
     </row>
     <row r="273">
-      <c r="A273" s="19" t="s">
+      <c r="A273" s="21" t="s">
         <v>272</v>
       </c>
       <c r="B273">
@@ -4376,7 +4380,7 @@
       </c>
     </row>
     <row r="274">
-      <c r="A274" s="19" t="s">
+      <c r="A274" s="21" t="s">
         <v>273</v>
       </c>
       <c r="B274">
@@ -4387,7 +4391,7 @@
       </c>
     </row>
     <row r="275">
-      <c r="A275" s="19" t="s">
+      <c r="A275" s="21" t="s">
         <v>274</v>
       </c>
       <c r="B275">
@@ -4398,7 +4402,7 @@
       </c>
     </row>
     <row r="276">
-      <c r="A276" s="19" t="s">
+      <c r="A276" s="21" t="s">
         <v>275</v>
       </c>
       <c r="B276">
@@ -4409,7 +4413,7 @@
       </c>
     </row>
     <row r="277">
-      <c r="A277" s="19" t="s">
+      <c r="A277" s="21" t="s">
         <v>276</v>
       </c>
       <c r="B277">
@@ -4420,7 +4424,7 @@
       </c>
     </row>
     <row r="278">
-      <c r="A278" s="19" t="s">
+      <c r="A278" s="21" t="s">
         <v>277</v>
       </c>
       <c r="B278">
@@ -4431,7 +4435,7 @@
       </c>
     </row>
     <row r="279">
-      <c r="A279" s="19" t="s">
+      <c r="A279" s="21" t="s">
         <v>278</v>
       </c>
       <c r="B279">
@@ -4442,7 +4446,7 @@
       </c>
     </row>
     <row r="280">
-      <c r="A280" s="19" t="s">
+      <c r="A280" s="21" t="s">
         <v>279</v>
       </c>
       <c r="B280">
@@ -4453,7 +4457,7 @@
       </c>
     </row>
     <row r="281">
-      <c r="A281" s="19" t="s">
+      <c r="A281" s="21" t="s">
         <v>280</v>
       </c>
       <c r="B281">
@@ -4464,7 +4468,7 @@
       </c>
     </row>
     <row r="282">
-      <c r="A282" s="19" t="s">
+      <c r="A282" s="21" t="s">
         <v>281</v>
       </c>
       <c r="B282">
@@ -4475,7 +4479,7 @@
       </c>
     </row>
     <row r="283">
-      <c r="A283" s="19" t="s">
+      <c r="A283" s="21" t="s">
         <v>282</v>
       </c>
       <c r="B283">
@@ -4486,7 +4490,7 @@
       </c>
     </row>
     <row r="284">
-      <c r="A284" s="19" t="s">
+      <c r="A284" s="21" t="s">
         <v>283</v>
       </c>
       <c r="B284">
@@ -4497,7 +4501,7 @@
       </c>
     </row>
     <row r="285">
-      <c r="A285" s="19" t="s">
+      <c r="A285" s="21" t="s">
         <v>284</v>
       </c>
       <c r="B285">
@@ -4508,7 +4512,7 @@
       </c>
     </row>
     <row r="286">
-      <c r="A286" s="19" t="s">
+      <c r="A286" s="21" t="s">
         <v>285</v>
       </c>
       <c r="B286">
@@ -4519,7 +4523,7 @@
       </c>
     </row>
     <row r="287">
-      <c r="A287" s="19" t="s">
+      <c r="A287" s="21" t="s">
         <v>286</v>
       </c>
       <c r="B287">
@@ -4530,7 +4534,7 @@
       </c>
     </row>
     <row r="288">
-      <c r="A288" s="19" t="s">
+      <c r="A288" s="21" t="s">
         <v>287</v>
       </c>
       <c r="B288">
@@ -4541,7 +4545,7 @@
       </c>
     </row>
     <row r="289">
-      <c r="A289" s="19" t="s">
+      <c r="A289" s="21" t="s">
         <v>288</v>
       </c>
       <c r="B289">
@@ -4552,7 +4556,7 @@
       </c>
     </row>
     <row r="290">
-      <c r="A290" s="19" t="s">
+      <c r="A290" s="21" t="s">
         <v>289</v>
       </c>
       <c r="B290">
@@ -4563,7 +4567,7 @@
       </c>
     </row>
     <row r="291">
-      <c r="A291" s="19" t="s">
+      <c r="A291" s="21" t="s">
         <v>290</v>
       </c>
       <c r="B291">
@@ -4574,7 +4578,7 @@
       </c>
     </row>
     <row r="292">
-      <c r="A292" s="19" t="s">
+      <c r="A292" s="21" t="s">
         <v>291</v>
       </c>
       <c r="B292">
@@ -4585,7 +4589,7 @@
       </c>
     </row>
     <row r="293">
-      <c r="A293" s="19" t="s">
+      <c r="A293" s="21" t="s">
         <v>292</v>
       </c>
       <c r="B293">
@@ -4596,7 +4600,7 @@
       </c>
     </row>
     <row r="294">
-      <c r="A294" s="19" t="s">
+      <c r="A294" s="21" t="s">
         <v>293</v>
       </c>
       <c r="B294">
@@ -4607,7 +4611,7 @@
       </c>
     </row>
     <row r="295">
-      <c r="A295" s="19" t="s">
+      <c r="A295" s="21" t="s">
         <v>294</v>
       </c>
       <c r="B295">
@@ -4618,7 +4622,7 @@
       </c>
     </row>
     <row r="296">
-      <c r="A296" s="19" t="s">
+      <c r="A296" s="21" t="s">
         <v>295</v>
       </c>
       <c r="B296">
@@ -4629,7 +4633,7 @@
       </c>
     </row>
     <row r="297">
-      <c r="A297" s="19" t="s">
+      <c r="A297" s="21" t="s">
         <v>296</v>
       </c>
       <c r="B297">
@@ -4640,7 +4644,7 @@
       </c>
     </row>
     <row r="298">
-      <c r="A298" s="19" t="s">
+      <c r="A298" s="21" t="s">
         <v>297</v>
       </c>
       <c r="B298">
@@ -4651,7 +4655,7 @@
       </c>
     </row>
     <row r="299">
-      <c r="A299" s="19" t="s">
+      <c r="A299" s="21" t="s">
         <v>298</v>
       </c>
       <c r="B299">
@@ -4662,7 +4666,7 @@
       </c>
     </row>
     <row r="300">
-      <c r="A300" s="19" t="s">
+      <c r="A300" s="21" t="s">
         <v>299</v>
       </c>
       <c r="B300">
@@ -4673,7 +4677,7 @@
       </c>
     </row>
     <row r="301">
-      <c r="A301" s="19" t="s">
+      <c r="A301" s="21" t="s">
         <v>300</v>
       </c>
       <c r="B301">
@@ -4684,7 +4688,7 @@
       </c>
     </row>
     <row r="302">
-      <c r="A302" s="19" t="s">
+      <c r="A302" s="21" t="s">
         <v>301</v>
       </c>
       <c r="B302">
@@ -4695,7 +4699,7 @@
       </c>
     </row>
     <row r="303">
-      <c r="A303" s="19" t="s">
+      <c r="A303" s="21" t="s">
         <v>302</v>
       </c>
       <c r="B303">
@@ -4706,7 +4710,7 @@
       </c>
     </row>
     <row r="304">
-      <c r="A304" s="19" t="s">
+      <c r="A304" s="21" t="s">
         <v>303</v>
       </c>
       <c r="B304">
@@ -4717,7 +4721,7 @@
       </c>
     </row>
     <row r="305">
-      <c r="A305" s="19" t="s">
+      <c r="A305" s="21" t="s">
         <v>304</v>
       </c>
       <c r="B305">
@@ -4728,7 +4732,7 @@
       </c>
     </row>
     <row r="306">
-      <c r="A306" s="19" t="s">
+      <c r="A306" s="21" t="s">
         <v>305</v>
       </c>
       <c r="B306">
@@ -4739,7 +4743,7 @@
       </c>
     </row>
     <row r="307">
-      <c r="A307" s="19" t="s">
+      <c r="A307" s="21" t="s">
         <v>306</v>
       </c>
       <c r="B307">
@@ -4750,7 +4754,7 @@
       </c>
     </row>
     <row r="308">
-      <c r="A308" s="19" t="s">
+      <c r="A308" s="21" t="s">
         <v>307</v>
       </c>
       <c r="B308">
@@ -4761,7 +4765,7 @@
       </c>
     </row>
     <row r="309">
-      <c r="A309" s="19" t="s">
+      <c r="A309" s="21" t="s">
         <v>308</v>
       </c>
       <c r="B309">
@@ -4772,7 +4776,7 @@
       </c>
     </row>
     <row r="310">
-      <c r="A310" s="19" t="s">
+      <c r="A310" s="21" t="s">
         <v>309</v>
       </c>
       <c r="B310">
@@ -4783,7 +4787,7 @@
       </c>
     </row>
     <row r="311">
-      <c r="A311" s="19" t="s">
+      <c r="A311" s="21" t="s">
         <v>310</v>
       </c>
       <c r="B311">
@@ -4794,7 +4798,7 @@
       </c>
     </row>
     <row r="312">
-      <c r="A312" s="19" t="s">
+      <c r="A312" s="21" t="s">
         <v>311</v>
       </c>
       <c r="B312">
@@ -4805,7 +4809,7 @@
       </c>
     </row>
     <row r="313">
-      <c r="A313" s="19" t="s">
+      <c r="A313" s="21" t="s">
         <v>312</v>
       </c>
       <c r="B313">
@@ -4816,7 +4820,7 @@
       </c>
     </row>
     <row r="314">
-      <c r="A314" s="19" t="s">
+      <c r="A314" s="21" t="s">
         <v>313</v>
       </c>
       <c r="B314">
@@ -4827,7 +4831,7 @@
       </c>
     </row>
     <row r="315">
-      <c r="A315" s="19" t="s">
+      <c r="A315" s="21" t="s">
         <v>314</v>
       </c>
       <c r="B315">
@@ -4838,7 +4842,7 @@
       </c>
     </row>
     <row r="316">
-      <c r="A316" s="19" t="s">
+      <c r="A316" s="21" t="s">
         <v>315</v>
       </c>
       <c r="B316">
@@ -4849,7 +4853,7 @@
       </c>
     </row>
     <row r="317">
-      <c r="A317" s="19" t="s">
+      <c r="A317" s="21" t="s">
         <v>316</v>
       </c>
       <c r="B317">
@@ -4860,7 +4864,7 @@
       </c>
     </row>
     <row r="318">
-      <c r="A318" s="19" t="s">
+      <c r="A318" s="21" t="s">
         <v>317</v>
       </c>
       <c r="B318">
@@ -4871,7 +4875,7 @@
       </c>
     </row>
     <row r="319">
-      <c r="A319" s="19" t="s">
+      <c r="A319" s="21" t="s">
         <v>318</v>
       </c>
       <c r="B319">
@@ -4882,7 +4886,7 @@
       </c>
     </row>
     <row r="320">
-      <c r="A320" s="19" t="s">
+      <c r="A320" s="21" t="s">
         <v>319</v>
       </c>
       <c r="B320">
@@ -4893,7 +4897,7 @@
       </c>
     </row>
     <row r="321">
-      <c r="A321" s="19" t="s">
+      <c r="A321" s="21" t="s">
         <v>320</v>
       </c>
       <c r="B321">
@@ -4904,7 +4908,7 @@
       </c>
     </row>
     <row r="322">
-      <c r="A322" s="19" t="s">
+      <c r="A322" s="21" t="s">
         <v>321</v>
       </c>
       <c r="B322">
@@ -4915,7 +4919,7 @@
       </c>
     </row>
     <row r="323">
-      <c r="A323" s="19" t="s">
+      <c r="A323" s="21" t="s">
         <v>322</v>
       </c>
       <c r="B323">
@@ -4926,7 +4930,7 @@
       </c>
     </row>
     <row r="324">
-      <c r="A324" s="19" t="s">
+      <c r="A324" s="21" t="s">
         <v>323</v>
       </c>
       <c r="B324">
@@ -4937,7 +4941,7 @@
       </c>
     </row>
     <row r="325">
-      <c r="A325" s="19" t="s">
+      <c r="A325" s="21" t="s">
         <v>324</v>
       </c>
       <c r="B325">
@@ -4948,7 +4952,7 @@
       </c>
     </row>
     <row r="326">
-      <c r="A326" s="19" t="s">
+      <c r="A326" s="21" t="s">
         <v>325</v>
       </c>
       <c r="B326">
@@ -4959,7 +4963,7 @@
       </c>
     </row>
     <row r="327">
-      <c r="A327" s="19" t="s">
+      <c r="A327" s="21" t="s">
         <v>326</v>
       </c>
       <c r="B327">
@@ -4970,7 +4974,7 @@
       </c>
     </row>
     <row r="328">
-      <c r="A328" s="19" t="s">
+      <c r="A328" s="21" t="s">
         <v>327</v>
       </c>
       <c r="B328">
@@ -4981,7 +4985,7 @@
       </c>
     </row>
     <row r="329">
-      <c r="A329" s="19" t="s">
+      <c r="A329" s="21" t="s">
         <v>328</v>
       </c>
       <c r="B329">
@@ -4992,7 +4996,7 @@
       </c>
     </row>
     <row r="330">
-      <c r="A330" s="19" t="s">
+      <c r="A330" s="21" t="s">
         <v>329</v>
       </c>
       <c r="B330">
@@ -5003,7 +5007,7 @@
       </c>
     </row>
     <row r="331">
-      <c r="A331" s="19" t="s">
+      <c r="A331" s="21" t="s">
         <v>330</v>
       </c>
       <c r="B331">
@@ -5014,7 +5018,7 @@
       </c>
     </row>
     <row r="332">
-      <c r="A332" s="19" t="s">
+      <c r="A332" s="21" t="s">
         <v>331</v>
       </c>
       <c r="B332">
@@ -5025,7 +5029,7 @@
       </c>
     </row>
     <row r="333">
-      <c r="A333" s="19" t="s">
+      <c r="A333" s="21" t="s">
         <v>332</v>
       </c>
       <c r="B333">
@@ -5036,7 +5040,7 @@
       </c>
     </row>
     <row r="334">
-      <c r="A334" s="19" t="s">
+      <c r="A334" s="21" t="s">
         <v>333</v>
       </c>
       <c r="B334">
@@ -5047,7 +5051,7 @@
       </c>
     </row>
     <row r="335">
-      <c r="A335" s="19" t="s">
+      <c r="A335" s="21" t="s">
         <v>334</v>
       </c>
       <c r="B335">
@@ -5058,7 +5062,7 @@
       </c>
     </row>
     <row r="336">
-      <c r="A336" s="19" t="s">
+      <c r="A336" s="21" t="s">
         <v>335</v>
       </c>
       <c r="B336">
@@ -5069,7 +5073,7 @@
       </c>
     </row>
     <row r="337">
-      <c r="A337" s="19" t="s">
+      <c r="A337" s="21" t="s">
         <v>336</v>
       </c>
       <c r="B337">
@@ -5080,7 +5084,7 @@
       </c>
     </row>
     <row r="338">
-      <c r="A338" s="19" t="s">
+      <c r="A338" s="21" t="s">
         <v>337</v>
       </c>
       <c r="B338">
@@ -5091,7 +5095,7 @@
       </c>
     </row>
     <row r="339">
-      <c r="A339" s="19" t="s">
+      <c r="A339" s="21" t="s">
         <v>338</v>
       </c>
       <c r="B339">
@@ -5102,7 +5106,7 @@
       </c>
     </row>
     <row r="340">
-      <c r="A340" s="19" t="s">
+      <c r="A340" s="21" t="s">
         <v>339</v>
       </c>
       <c r="B340">
@@ -5113,7 +5117,7 @@
       </c>
     </row>
     <row r="341">
-      <c r="A341" s="19" t="s">
+      <c r="A341" s="21" t="s">
         <v>340</v>
       </c>
       <c r="B341">
@@ -5124,7 +5128,7 @@
       </c>
     </row>
     <row r="342">
-      <c r="A342" s="19" t="s">
+      <c r="A342" s="21" t="s">
         <v>341</v>
       </c>
       <c r="B342">
@@ -5135,7 +5139,7 @@
       </c>
     </row>
     <row r="343">
-      <c r="A343" s="19" t="s">
+      <c r="A343" s="21" t="s">
         <v>342</v>
       </c>
       <c r="B343">
@@ -5146,7 +5150,7 @@
       </c>
     </row>
     <row r="344">
-      <c r="A344" s="19" t="s">
+      <c r="A344" s="21" t="s">
         <v>343</v>
       </c>
       <c r="B344">
@@ -5157,7 +5161,7 @@
       </c>
     </row>
     <row r="345">
-      <c r="A345" s="19" t="s">
+      <c r="A345" s="21" t="s">
         <v>344</v>
       </c>
       <c r="B345">
@@ -5168,7 +5172,7 @@
       </c>
     </row>
     <row r="346">
-      <c r="A346" s="19" t="s">
+      <c r="A346" s="21" t="s">
         <v>345</v>
       </c>
       <c r="B346">
@@ -5179,7 +5183,7 @@
       </c>
     </row>
     <row r="347">
-      <c r="A347" s="19" t="s">
+      <c r="A347" s="21" t="s">
         <v>346</v>
       </c>
       <c r="B347">
@@ -5190,7 +5194,7 @@
       </c>
     </row>
     <row r="348">
-      <c r="A348" s="19" t="s">
+      <c r="A348" s="21" t="s">
         <v>347</v>
       </c>
       <c r="B348">
@@ -5201,7 +5205,7 @@
       </c>
     </row>
     <row r="349">
-      <c r="A349" s="19" t="s">
+      <c r="A349" s="21" t="s">
         <v>348</v>
       </c>
       <c r="B349">
@@ -5212,7 +5216,7 @@
       </c>
     </row>
     <row r="350">
-      <c r="A350" s="19" t="s">
+      <c r="A350" s="21" t="s">
         <v>349</v>
       </c>
       <c r="B350">
@@ -5223,7 +5227,7 @@
       </c>
     </row>
     <row r="351">
-      <c r="A351" s="19" t="s">
+      <c r="A351" s="21" t="s">
         <v>350</v>
       </c>
       <c r="B351">
@@ -5234,7 +5238,7 @@
       </c>
     </row>
     <row r="352">
-      <c r="A352" s="19" t="s">
+      <c r="A352" s="21" t="s">
         <v>351</v>
       </c>
       <c r="B352">
@@ -5245,7 +5249,7 @@
       </c>
     </row>
     <row r="353">
-      <c r="A353" s="19" t="s">
+      <c r="A353" s="21" t="s">
         <v>352</v>
       </c>
       <c r="B353">
@@ -5256,7 +5260,7 @@
       </c>
     </row>
     <row r="354">
-      <c r="A354" s="19" t="s">
+      <c r="A354" s="21" t="s">
         <v>353</v>
       </c>
       <c r="B354">
@@ -5267,7 +5271,7 @@
       </c>
     </row>
     <row r="355">
-      <c r="A355" s="19" t="s">
+      <c r="A355" s="21" t="s">
         <v>354</v>
       </c>
       <c r="B355">
@@ -5278,7 +5282,7 @@
       </c>
     </row>
     <row r="356">
-      <c r="A356" s="19" t="s">
+      <c r="A356" s="21" t="s">
         <v>355</v>
       </c>
       <c r="B356">
@@ -5289,7 +5293,7 @@
       </c>
     </row>
     <row r="357">
-      <c r="A357" s="19" t="s">
+      <c r="A357" s="21" t="s">
         <v>356</v>
       </c>
       <c r="B357">
@@ -5300,7 +5304,7 @@
       </c>
     </row>
     <row r="358">
-      <c r="A358" s="19" t="s">
+      <c r="A358" s="21" t="s">
         <v>357</v>
       </c>
       <c r="B358">
@@ -5311,7 +5315,7 @@
       </c>
     </row>
     <row r="359">
-      <c r="A359" s="19" t="s">
+      <c r="A359" s="21" t="s">
         <v>358</v>
       </c>
       <c r="B359">
@@ -5322,7 +5326,7 @@
       </c>
     </row>
     <row r="360">
-      <c r="A360" s="19" t="s">
+      <c r="A360" s="21" t="s">
         <v>359</v>
       </c>
       <c r="B360">
@@ -5333,7 +5337,7 @@
       </c>
     </row>
     <row r="361">
-      <c r="A361" s="19" t="s">
+      <c r="A361" s="21" t="s">
         <v>360</v>
       </c>
       <c r="B361">
@@ -5344,7 +5348,7 @@
       </c>
     </row>
     <row r="362">
-      <c r="A362" s="19" t="s">
+      <c r="A362" s="21" t="s">
         <v>361</v>
       </c>
       <c r="B362">
@@ -5355,7 +5359,7 @@
       </c>
     </row>
     <row r="363">
-      <c r="A363" s="19" t="s">
+      <c r="A363" s="21" t="s">
         <v>362</v>
       </c>
       <c r="B363">
@@ -5366,7 +5370,7 @@
       </c>
     </row>
     <row r="364">
-      <c r="A364" s="19" t="s">
+      <c r="A364" s="21" t="s">
         <v>363</v>
       </c>
       <c r="B364">
@@ -5377,7 +5381,7 @@
       </c>
     </row>
     <row r="365">
-      <c r="A365" s="19" t="s">
+      <c r="A365" s="21" t="s">
         <v>364</v>
       </c>
       <c r="B365">
@@ -5388,7 +5392,7 @@
       </c>
     </row>
     <row r="366">
-      <c r="A366" s="19" t="s">
+      <c r="A366" s="21" t="s">
         <v>365</v>
       </c>
       <c r="B366">
@@ -5399,7 +5403,7 @@
       </c>
     </row>
     <row r="367">
-      <c r="A367" s="19" t="s">
+      <c r="A367" s="21" t="s">
         <v>366</v>
       </c>
       <c r="B367">
@@ -5410,7 +5414,7 @@
       </c>
     </row>
     <row r="368">
-      <c r="A368" s="19" t="s">
+      <c r="A368" s="21" t="s">
         <v>367</v>
       </c>
       <c r="B368">
@@ -5421,7 +5425,7 @@
       </c>
     </row>
     <row r="369">
-      <c r="A369" s="19" t="s">
+      <c r="A369" s="21" t="s">
         <v>368</v>
       </c>
       <c r="B369">
@@ -5432,7 +5436,7 @@
       </c>
     </row>
     <row r="370">
-      <c r="A370" s="19" t="s">
+      <c r="A370" s="21" t="s">
         <v>369</v>
       </c>
       <c r="B370">
@@ -5443,7 +5447,7 @@
       </c>
     </row>
     <row r="371">
-      <c r="A371" s="19" t="s">
+      <c r="A371" s="21" t="s">
         <v>370</v>
       </c>
       <c r="B371">
@@ -5454,7 +5458,7 @@
       </c>
     </row>
     <row r="372">
-      <c r="A372" s="19" t="s">
+      <c r="A372" s="21" t="s">
         <v>371</v>
       </c>
       <c r="B372">
@@ -5465,7 +5469,7 @@
       </c>
     </row>
     <row r="373">
-      <c r="A373" s="19" t="s">
+      <c r="A373" s="21" t="s">
         <v>372</v>
       </c>
       <c r="B373">
@@ -5476,7 +5480,7 @@
       </c>
     </row>
     <row r="374">
-      <c r="A374" s="19" t="s">
+      <c r="A374" s="21" t="s">
         <v>373</v>
       </c>
       <c r="B374">
@@ -5487,7 +5491,7 @@
       </c>
     </row>
     <row r="375">
-      <c r="A375" s="19" t="s">
+      <c r="A375" s="21" t="s">
         <v>374</v>
       </c>
       <c r="B375">
@@ -5498,7 +5502,7 @@
       </c>
     </row>
     <row r="376">
-      <c r="A376" s="19" t="s">
+      <c r="A376" s="21" t="s">
         <v>375</v>
       </c>
       <c r="B376">
@@ -5509,7 +5513,7 @@
       </c>
     </row>
     <row r="377">
-      <c r="A377" s="19" t="s">
+      <c r="A377" s="21" t="s">
         <v>376</v>
       </c>
       <c r="B377">
@@ -5520,7 +5524,7 @@
       </c>
     </row>
     <row r="378">
-      <c r="A378" s="19" t="s">
+      <c r="A378" s="21" t="s">
         <v>377</v>
       </c>
       <c r="B378">
@@ -5531,7 +5535,7 @@
       </c>
     </row>
     <row r="379">
-      <c r="A379" s="19" t="s">
+      <c r="A379" s="21" t="s">
         <v>378</v>
       </c>
       <c r="B379">
@@ -5542,7 +5546,7 @@
       </c>
     </row>
     <row r="380">
-      <c r="A380" s="19" t="s">
+      <c r="A380" s="21" t="s">
         <v>379</v>
       </c>
       <c r="B380">
@@ -5553,7 +5557,7 @@
       </c>
     </row>
     <row r="381">
-      <c r="A381" s="19" t="s">
+      <c r="A381" s="21" t="s">
         <v>380</v>
       </c>
       <c r="B381">
@@ -5564,7 +5568,7 @@
       </c>
     </row>
     <row r="382">
-      <c r="A382" s="19" t="s">
+      <c r="A382" s="21" t="s">
         <v>381</v>
       </c>
       <c r="B382">
@@ -5575,7 +5579,7 @@
       </c>
     </row>
     <row r="383">
-      <c r="A383" s="19" t="s">
+      <c r="A383" s="21" t="s">
         <v>382</v>
       </c>
       <c r="B383">
@@ -5586,7 +5590,7 @@
       </c>
     </row>
     <row r="384">
-      <c r="A384" s="19" t="s">
+      <c r="A384" s="21" t="s">
         <v>383</v>
       </c>
       <c r="B384">
@@ -5597,7 +5601,7 @@
       </c>
     </row>
     <row r="385">
-      <c r="A385" s="19" t="s">
+      <c r="A385" s="21" t="s">
         <v>384</v>
       </c>
       <c r="B385">
@@ -5608,7 +5612,7 @@
       </c>
     </row>
     <row r="386">
-      <c r="A386" s="19" t="s">
+      <c r="A386" s="21" t="s">
         <v>385</v>
       </c>
       <c r="B386">
@@ -5619,7 +5623,7 @@
       </c>
     </row>
     <row r="387">
-      <c r="A387" s="19" t="s">
+      <c r="A387" s="21" t="s">
         <v>386</v>
       </c>
       <c r="B387">
@@ -5630,7 +5634,7 @@
       </c>
     </row>
     <row r="388">
-      <c r="A388" s="19" t="s">
+      <c r="A388" s="21" t="s">
         <v>387</v>
       </c>
       <c r="B388">
@@ -5641,7 +5645,7 @@
       </c>
     </row>
     <row r="389">
-      <c r="A389" s="19" t="s">
+      <c r="A389" s="21" t="s">
         <v>388</v>
       </c>
       <c r="B389">
@@ -5652,7 +5656,7 @@
       </c>
     </row>
     <row r="390">
-      <c r="A390" s="19" t="s">
+      <c r="A390" s="21" t="s">
         <v>389</v>
       </c>
       <c r="B390">
@@ -5663,7 +5667,7 @@
       </c>
     </row>
     <row r="391">
-      <c r="A391" s="19" t="s">
+      <c r="A391" s="21" t="s">
         <v>390</v>
       </c>
       <c r="B391">
@@ -5674,7 +5678,7 @@
       </c>
     </row>
     <row r="392">
-      <c r="A392" s="19" t="s">
+      <c r="A392" s="21" t="s">
         <v>391</v>
       </c>
       <c r="B392">
@@ -5685,7 +5689,7 @@
       </c>
     </row>
     <row r="393">
-      <c r="A393" s="19" t="s">
+      <c r="A393" s="21" t="s">
         <v>392</v>
       </c>
       <c r="B393">
@@ -5696,7 +5700,7 @@
       </c>
     </row>
     <row r="394">
-      <c r="A394" s="19" t="s">
+      <c r="A394" s="21" t="s">
         <v>393</v>
       </c>
       <c r="B394">
@@ -5707,7 +5711,7 @@
       </c>
     </row>
     <row r="395">
-      <c r="A395" s="19" t="s">
+      <c r="A395" s="21" t="s">
         <v>394</v>
       </c>
       <c r="B395">
@@ -5718,7 +5722,7 @@
       </c>
     </row>
     <row r="396">
-      <c r="A396" s="19" t="s">
+      <c r="A396" s="21" t="s">
         <v>395</v>
       </c>
       <c r="B396">
@@ -5729,7 +5733,7 @@
       </c>
     </row>
     <row r="397">
-      <c r="A397" s="19" t="s">
+      <c r="A397" s="21" t="s">
         <v>396</v>
       </c>
       <c r="B397">
@@ -5740,7 +5744,7 @@
       </c>
     </row>
     <row r="398">
-      <c r="A398" s="19" t="s">
+      <c r="A398" s="21" t="s">
         <v>397</v>
       </c>
       <c r="B398">
@@ -5751,7 +5755,7 @@
       </c>
     </row>
     <row r="399">
-      <c r="A399" s="19" t="s">
+      <c r="A399" s="21" t="s">
         <v>398</v>
       </c>
       <c r="B399">
@@ -5762,7 +5766,7 @@
       </c>
     </row>
     <row r="400">
-      <c r="A400" s="19" t="s">
+      <c r="A400" s="21" t="s">
         <v>399</v>
       </c>
       <c r="B400">
@@ -5773,7 +5777,7 @@
       </c>
     </row>
     <row r="401">
-      <c r="A401" s="19" t="s">
+      <c r="A401" s="21" t="s">
         <v>400</v>
       </c>
       <c r="B401">
@@ -5784,7 +5788,7 @@
       </c>
     </row>
     <row r="402">
-      <c r="A402" s="19" t="s">
+      <c r="A402" s="21" t="s">
         <v>401</v>
       </c>
       <c r="B402">
@@ -5795,7 +5799,7 @@
       </c>
     </row>
     <row r="403">
-      <c r="A403" s="19" t="s">
+      <c r="A403" s="21" t="s">
         <v>402</v>
       </c>
       <c r="B403">
@@ -5806,7 +5810,7 @@
       </c>
     </row>
     <row r="404">
-      <c r="A404" s="19" t="s">
+      <c r="A404" s="21" t="s">
         <v>403</v>
       </c>
       <c r="B404">
@@ -5817,7 +5821,7 @@
       </c>
     </row>
     <row r="405">
-      <c r="A405" s="19" t="s">
+      <c r="A405" s="21" t="s">
         <v>404</v>
       </c>
       <c r="B405">
@@ -5828,7 +5832,7 @@
       </c>
     </row>
     <row r="406">
-      <c r="A406" s="19" t="s">
+      <c r="A406" s="21" t="s">
         <v>405</v>
       </c>
       <c r="B406">
@@ -5839,7 +5843,7 @@
       </c>
     </row>
     <row r="407">
-      <c r="A407" s="19" t="s">
+      <c r="A407" s="21" t="s">
         <v>406</v>
       </c>
       <c r="B407">
@@ -5850,7 +5854,7 @@
       </c>
     </row>
     <row r="408">
-      <c r="A408" s="19" t="s">
+      <c r="A408" s="21" t="s">
         <v>407</v>
       </c>
       <c r="B408">
@@ -5861,7 +5865,7 @@
       </c>
     </row>
     <row r="409">
-      <c r="A409" s="19" t="s">
+      <c r="A409" s="21" t="s">
         <v>408</v>
       </c>
       <c r="B409">
@@ -5872,7 +5876,7 @@
       </c>
     </row>
     <row r="410">
-      <c r="A410" s="19" t="s">
+      <c r="A410" s="21" t="s">
         <v>409</v>
       </c>
       <c r="B410">
@@ -5883,7 +5887,7 @@
       </c>
     </row>
     <row r="411">
-      <c r="A411" s="19" t="s">
+      <c r="A411" s="21" t="s">
         <v>410</v>
       </c>
       <c r="B411">
@@ -5894,7 +5898,7 @@
       </c>
     </row>
     <row r="412">
-      <c r="A412" s="19" t="s">
+      <c r="A412" s="21" t="s">
         <v>411</v>
       </c>
       <c r="B412">
@@ -5905,7 +5909,7 @@
       </c>
     </row>
     <row r="413">
-      <c r="A413" s="19" t="s">
+      <c r="A413" s="21" t="s">
         <v>412</v>
       </c>
       <c r="B413">
@@ -5916,7 +5920,7 @@
       </c>
     </row>
     <row r="414">
-      <c r="A414" s="19" t="s">
+      <c r="A414" s="21" t="s">
         <v>413</v>
       </c>
       <c r="B414">
@@ -5927,7 +5931,7 @@
       </c>
     </row>
     <row r="415">
-      <c r="A415" s="19" t="s">
+      <c r="A415" s="21" t="s">
         <v>414</v>
       </c>
       <c r="B415">
@@ -5938,7 +5942,7 @@
       </c>
     </row>
     <row r="416">
-      <c r="A416" s="19" t="s">
+      <c r="A416" s="21" t="s">
         <v>415</v>
       </c>
       <c r="B416">
@@ -5949,7 +5953,7 @@
       </c>
     </row>
     <row r="417">
-      <c r="A417" s="19" t="s">
+      <c r="A417" s="21" t="s">
         <v>416</v>
       </c>
       <c r="B417">
@@ -5960,7 +5964,7 @@
       </c>
     </row>
     <row r="418">
-      <c r="A418" s="19" t="s">
+      <c r="A418" s="21" t="s">
         <v>417</v>
       </c>
       <c r="B418">
@@ -5971,7 +5975,7 @@
       </c>
     </row>
     <row r="419">
-      <c r="A419" s="19" t="s">
+      <c r="A419" s="21" t="s">
         <v>418</v>
       </c>
       <c r="B419">
@@ -5982,7 +5986,7 @@
       </c>
     </row>
     <row r="420">
-      <c r="A420" s="19" t="s">
+      <c r="A420" s="21" t="s">
         <v>419</v>
       </c>
       <c r="B420">

</xml_diff>

<commit_message>
Increase image resolution for paper
</commit_message>
<xml_diff>
--- a/results/results_drug_on_mutation_of_Ras.xlsx
+++ b/results/results_drug_on_mutation_of_Ras.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8862" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14770" uniqueCount="422">
   <si>
     <t>Protein</t>
   </si>
@@ -1301,7 +1301,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="71">
     <border>
       <left/>
       <right/>
@@ -1351,11 +1351,39 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1399,6 +1427,34 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="67" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="68" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="69" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="70" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1417,18 +1473,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="41" t="s">
+      <c r="A1" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="69" t="s">
         <v>420</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="69" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="69" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -1439,7 +1495,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="69" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -1450,7 +1506,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="69" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -1461,7 +1517,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="69" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -1472,7 +1528,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="69" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -1483,7 +1539,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="69" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -1494,7 +1550,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="69" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -1505,7 +1561,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="69" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -1516,7 +1572,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="69" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -1527,7 +1583,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="69" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -1538,7 +1594,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="69" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -1549,7 +1605,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="69" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -1560,7 +1616,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="69" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -1571,7 +1627,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="69" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -1582,7 +1638,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="69" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -1593,7 +1649,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="69" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -1604,7 +1660,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="69" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -1615,7 +1671,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="69" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -1626,7 +1682,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="69" t="s">
         <v>19</v>
       </c>
       <c r="B20">
@@ -1637,7 +1693,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="69" t="s">
         <v>20</v>
       </c>
       <c r="B21">
@@ -1648,7 +1704,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="69" t="s">
         <v>21</v>
       </c>
       <c r="B22">
@@ -1659,7 +1715,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="69" t="s">
         <v>22</v>
       </c>
       <c r="B23">
@@ -1670,7 +1726,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="69" t="s">
         <v>23</v>
       </c>
       <c r="B24">
@@ -1681,7 +1737,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="69" t="s">
         <v>24</v>
       </c>
       <c r="B25">
@@ -1692,7 +1748,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="69" t="s">
         <v>25</v>
       </c>
       <c r="B26">
@@ -1703,7 +1759,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="69" t="s">
         <v>26</v>
       </c>
       <c r="B27">
@@ -1714,7 +1770,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="69" t="s">
         <v>27</v>
       </c>
       <c r="B28">
@@ -1725,7 +1781,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="69" t="s">
         <v>28</v>
       </c>
       <c r="B29">
@@ -1736,7 +1792,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="69" t="s">
         <v>29</v>
       </c>
       <c r="B30">
@@ -1747,7 +1803,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="69" t="s">
         <v>30</v>
       </c>
       <c r="B31">
@@ -1758,7 +1814,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="69" t="s">
         <v>31</v>
       </c>
       <c r="B32">
@@ -1769,7 +1825,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="69" t="s">
         <v>32</v>
       </c>
       <c r="B33">
@@ -1780,7 +1836,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="41" t="s">
+      <c r="A34" s="69" t="s">
         <v>33</v>
       </c>
       <c r="B34">
@@ -1791,7 +1847,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="69" t="s">
         <v>34</v>
       </c>
       <c r="B35">
@@ -1802,7 +1858,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="69" t="s">
         <v>35</v>
       </c>
       <c r="B36">
@@ -1813,7 +1869,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="41" t="s">
+      <c r="A37" s="69" t="s">
         <v>36</v>
       </c>
       <c r="B37">
@@ -1824,7 +1880,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="41" t="s">
+      <c r="A38" s="69" t="s">
         <v>37</v>
       </c>
       <c r="B38">
@@ -1835,7 +1891,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="41" t="s">
+      <c r="A39" s="69" t="s">
         <v>38</v>
       </c>
       <c r="B39">
@@ -1846,7 +1902,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="41" t="s">
+      <c r="A40" s="69" t="s">
         <v>39</v>
       </c>
       <c r="B40">
@@ -1857,7 +1913,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="41" t="s">
+      <c r="A41" s="69" t="s">
         <v>40</v>
       </c>
       <c r="B41">
@@ -1868,7 +1924,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="69" t="s">
         <v>41</v>
       </c>
       <c r="B42">
@@ -1879,7 +1935,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="41" t="s">
+      <c r="A43" s="69" t="s">
         <v>42</v>
       </c>
       <c r="B43">
@@ -1890,7 +1946,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="69" t="s">
         <v>43</v>
       </c>
       <c r="B44">
@@ -1901,7 +1957,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="69" t="s">
         <v>44</v>
       </c>
       <c r="B45">
@@ -1912,7 +1968,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="41" t="s">
+      <c r="A46" s="69" t="s">
         <v>45</v>
       </c>
       <c r="B46">
@@ -1923,7 +1979,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="69" t="s">
         <v>46</v>
       </c>
       <c r="B47">
@@ -1934,7 +1990,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="41" t="s">
+      <c r="A48" s="69" t="s">
         <v>47</v>
       </c>
       <c r="B48">
@@ -1945,7 +2001,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="41" t="s">
+      <c r="A49" s="69" t="s">
         <v>48</v>
       </c>
       <c r="B49">
@@ -1956,7 +2012,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="41" t="s">
+      <c r="A50" s="69" t="s">
         <v>49</v>
       </c>
       <c r="B50">
@@ -1967,7 +2023,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="41" t="s">
+      <c r="A51" s="69" t="s">
         <v>50</v>
       </c>
       <c r="B51">
@@ -1978,7 +2034,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="41" t="s">
+      <c r="A52" s="69" t="s">
         <v>51</v>
       </c>
       <c r="B52">
@@ -1989,7 +2045,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="41" t="s">
+      <c r="A53" s="69" t="s">
         <v>52</v>
       </c>
       <c r="B53">
@@ -2000,7 +2056,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="41" t="s">
+      <c r="A54" s="69" t="s">
         <v>53</v>
       </c>
       <c r="B54">
@@ -2011,7 +2067,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="41" t="s">
+      <c r="A55" s="69" t="s">
         <v>54</v>
       </c>
       <c r="B55">
@@ -2022,7 +2078,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="41" t="s">
+      <c r="A56" s="69" t="s">
         <v>55</v>
       </c>
       <c r="B56">
@@ -2033,7 +2089,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="41" t="s">
+      <c r="A57" s="69" t="s">
         <v>56</v>
       </c>
       <c r="B57">
@@ -2044,7 +2100,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="41" t="s">
+      <c r="A58" s="69" t="s">
         <v>57</v>
       </c>
       <c r="B58">
@@ -2055,7 +2111,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="41" t="s">
+      <c r="A59" s="69" t="s">
         <v>58</v>
       </c>
       <c r="B59">
@@ -2066,7 +2122,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="41" t="s">
+      <c r="A60" s="69" t="s">
         <v>59</v>
       </c>
       <c r="B60">
@@ -2077,7 +2133,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="41" t="s">
+      <c r="A61" s="69" t="s">
         <v>60</v>
       </c>
       <c r="B61">
@@ -2088,7 +2144,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="41" t="s">
+      <c r="A62" s="69" t="s">
         <v>61</v>
       </c>
       <c r="B62">
@@ -2099,7 +2155,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="41" t="s">
+      <c r="A63" s="69" t="s">
         <v>62</v>
       </c>
       <c r="B63">
@@ -2110,7 +2166,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="41" t="s">
+      <c r="A64" s="69" t="s">
         <v>63</v>
       </c>
       <c r="B64">
@@ -2121,7 +2177,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="41" t="s">
+      <c r="A65" s="69" t="s">
         <v>64</v>
       </c>
       <c r="B65">
@@ -2132,7 +2188,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="41" t="s">
+      <c r="A66" s="69" t="s">
         <v>65</v>
       </c>
       <c r="B66">
@@ -2143,7 +2199,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="41" t="s">
+      <c r="A67" s="69" t="s">
         <v>66</v>
       </c>
       <c r="B67">
@@ -2154,7 +2210,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="41" t="s">
+      <c r="A68" s="69" t="s">
         <v>67</v>
       </c>
       <c r="B68">
@@ -2165,7 +2221,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="41" t="s">
+      <c r="A69" s="69" t="s">
         <v>68</v>
       </c>
       <c r="B69">
@@ -2176,7 +2232,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="41" t="s">
+      <c r="A70" s="69" t="s">
         <v>69</v>
       </c>
       <c r="B70">
@@ -2187,7 +2243,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="41" t="s">
+      <c r="A71" s="69" t="s">
         <v>70</v>
       </c>
       <c r="B71">
@@ -2198,7 +2254,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="41" t="s">
+      <c r="A72" s="69" t="s">
         <v>71</v>
       </c>
       <c r="B72">
@@ -2209,7 +2265,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="41" t="s">
+      <c r="A73" s="69" t="s">
         <v>72</v>
       </c>
       <c r="B73">
@@ -2220,7 +2276,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="41" t="s">
+      <c r="A74" s="69" t="s">
         <v>73</v>
       </c>
       <c r="B74">
@@ -2231,7 +2287,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="41" t="s">
+      <c r="A75" s="69" t="s">
         <v>74</v>
       </c>
       <c r="B75">
@@ -2242,7 +2298,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="41" t="s">
+      <c r="A76" s="69" t="s">
         <v>75</v>
       </c>
       <c r="B76">
@@ -2253,7 +2309,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="41" t="s">
+      <c r="A77" s="69" t="s">
         <v>76</v>
       </c>
       <c r="B77">
@@ -2264,7 +2320,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="41" t="s">
+      <c r="A78" s="69" t="s">
         <v>77</v>
       </c>
       <c r="B78">
@@ -2275,7 +2331,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="41" t="s">
+      <c r="A79" s="69" t="s">
         <v>78</v>
       </c>
       <c r="B79">
@@ -2286,7 +2342,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="41" t="s">
+      <c r="A80" s="69" t="s">
         <v>79</v>
       </c>
       <c r="B80">
@@ -2297,7 +2353,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="41" t="s">
+      <c r="A81" s="69" t="s">
         <v>80</v>
       </c>
       <c r="B81">
@@ -2308,7 +2364,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="41" t="s">
+      <c r="A82" s="69" t="s">
         <v>81</v>
       </c>
       <c r="B82">
@@ -2319,7 +2375,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="41" t="s">
+      <c r="A83" s="69" t="s">
         <v>82</v>
       </c>
       <c r="B83">
@@ -2330,7 +2386,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="41" t="s">
+      <c r="A84" s="69" t="s">
         <v>83</v>
       </c>
       <c r="B84">
@@ -2341,7 +2397,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="41" t="s">
+      <c r="A85" s="69" t="s">
         <v>84</v>
       </c>
       <c r="B85">
@@ -2352,7 +2408,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="41" t="s">
+      <c r="A86" s="69" t="s">
         <v>85</v>
       </c>
       <c r="B86">
@@ -2363,7 +2419,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="41" t="s">
+      <c r="A87" s="69" t="s">
         <v>86</v>
       </c>
       <c r="B87">
@@ -2374,7 +2430,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="41" t="s">
+      <c r="A88" s="69" t="s">
         <v>87</v>
       </c>
       <c r="B88">
@@ -2385,7 +2441,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="41" t="s">
+      <c r="A89" s="69" t="s">
         <v>88</v>
       </c>
       <c r="B89">
@@ -2396,7 +2452,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="41" t="s">
+      <c r="A90" s="69" t="s">
         <v>89</v>
       </c>
       <c r="B90">
@@ -2407,7 +2463,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="41" t="s">
+      <c r="A91" s="69" t="s">
         <v>90</v>
       </c>
       <c r="B91">
@@ -2418,7 +2474,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="41" t="s">
+      <c r="A92" s="69" t="s">
         <v>91</v>
       </c>
       <c r="B92">
@@ -2429,7 +2485,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="41" t="s">
+      <c r="A93" s="69" t="s">
         <v>92</v>
       </c>
       <c r="B93">
@@ -2440,7 +2496,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="41" t="s">
+      <c r="A94" s="69" t="s">
         <v>93</v>
       </c>
       <c r="B94">
@@ -2451,7 +2507,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="41" t="s">
+      <c r="A95" s="69" t="s">
         <v>94</v>
       </c>
       <c r="B95">
@@ -2462,7 +2518,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="41" t="s">
+      <c r="A96" s="69" t="s">
         <v>95</v>
       </c>
       <c r="B96">
@@ -2473,7 +2529,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="41" t="s">
+      <c r="A97" s="69" t="s">
         <v>96</v>
       </c>
       <c r="B97">
@@ -2484,7 +2540,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="41" t="s">
+      <c r="A98" s="69" t="s">
         <v>97</v>
       </c>
       <c r="B98">
@@ -2495,7 +2551,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="41" t="s">
+      <c r="A99" s="69" t="s">
         <v>98</v>
       </c>
       <c r="B99">
@@ -2506,7 +2562,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="41" t="s">
+      <c r="A100" s="69" t="s">
         <v>99</v>
       </c>
       <c r="B100">
@@ -2517,7 +2573,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="41" t="s">
+      <c r="A101" s="69" t="s">
         <v>100</v>
       </c>
       <c r="B101">
@@ -2528,7 +2584,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="41" t="s">
+      <c r="A102" s="69" t="s">
         <v>101</v>
       </c>
       <c r="B102">
@@ -2539,7 +2595,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="41" t="s">
+      <c r="A103" s="69" t="s">
         <v>102</v>
       </c>
       <c r="B103">
@@ -2550,7 +2606,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="41" t="s">
+      <c r="A104" s="69" t="s">
         <v>103</v>
       </c>
       <c r="B104">
@@ -2561,7 +2617,7 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="41" t="s">
+      <c r="A105" s="69" t="s">
         <v>104</v>
       </c>
       <c r="B105">
@@ -2572,7 +2628,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="41" t="s">
+      <c r="A106" s="69" t="s">
         <v>105</v>
       </c>
       <c r="B106">
@@ -2583,7 +2639,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="41" t="s">
+      <c r="A107" s="69" t="s">
         <v>106</v>
       </c>
       <c r="B107">
@@ -2594,7 +2650,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="41" t="s">
+      <c r="A108" s="69" t="s">
         <v>107</v>
       </c>
       <c r="B108">
@@ -2605,7 +2661,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="41" t="s">
+      <c r="A109" s="69" t="s">
         <v>108</v>
       </c>
       <c r="B109">
@@ -2616,7 +2672,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="41" t="s">
+      <c r="A110" s="69" t="s">
         <v>109</v>
       </c>
       <c r="B110">
@@ -2627,7 +2683,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="41" t="s">
+      <c r="A111" s="69" t="s">
         <v>110</v>
       </c>
       <c r="B111">
@@ -2638,7 +2694,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="41" t="s">
+      <c r="A112" s="69" t="s">
         <v>111</v>
       </c>
       <c r="B112">
@@ -2649,7 +2705,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="41" t="s">
+      <c r="A113" s="69" t="s">
         <v>112</v>
       </c>
       <c r="B113">
@@ -2660,7 +2716,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="41" t="s">
+      <c r="A114" s="69" t="s">
         <v>113</v>
       </c>
       <c r="B114">
@@ -2671,7 +2727,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="41" t="s">
+      <c r="A115" s="69" t="s">
         <v>114</v>
       </c>
       <c r="B115">
@@ -2682,7 +2738,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="41" t="s">
+      <c r="A116" s="69" t="s">
         <v>115</v>
       </c>
       <c r="B116">
@@ -2693,7 +2749,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="41" t="s">
+      <c r="A117" s="69" t="s">
         <v>116</v>
       </c>
       <c r="B117">
@@ -2704,7 +2760,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="41" t="s">
+      <c r="A118" s="69" t="s">
         <v>117</v>
       </c>
       <c r="B118">
@@ -2715,7 +2771,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="41" t="s">
+      <c r="A119" s="69" t="s">
         <v>118</v>
       </c>
       <c r="B119">
@@ -2726,7 +2782,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="41" t="s">
+      <c r="A120" s="69" t="s">
         <v>119</v>
       </c>
       <c r="B120">
@@ -2737,7 +2793,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="41" t="s">
+      <c r="A121" s="69" t="s">
         <v>120</v>
       </c>
       <c r="B121">
@@ -2748,7 +2804,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="41" t="s">
+      <c r="A122" s="69" t="s">
         <v>121</v>
       </c>
       <c r="B122">
@@ -2759,7 +2815,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="41" t="s">
+      <c r="A123" s="69" t="s">
         <v>122</v>
       </c>
       <c r="B123">
@@ -2770,7 +2826,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="41" t="s">
+      <c r="A124" s="69" t="s">
         <v>123</v>
       </c>
       <c r="B124">
@@ -2781,7 +2837,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="41" t="s">
+      <c r="A125" s="69" t="s">
         <v>124</v>
       </c>
       <c r="B125">
@@ -2792,7 +2848,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="41" t="s">
+      <c r="A126" s="69" t="s">
         <v>125</v>
       </c>
       <c r="B126">
@@ -2803,7 +2859,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="41" t="s">
+      <c r="A127" s="69" t="s">
         <v>126</v>
       </c>
       <c r="B127">
@@ -2814,7 +2870,7 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="41" t="s">
+      <c r="A128" s="69" t="s">
         <v>127</v>
       </c>
       <c r="B128">
@@ -2825,7 +2881,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="41" t="s">
+      <c r="A129" s="69" t="s">
         <v>128</v>
       </c>
       <c r="B129">
@@ -2836,7 +2892,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="41" t="s">
+      <c r="A130" s="69" t="s">
         <v>129</v>
       </c>
       <c r="B130">
@@ -2847,7 +2903,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="41" t="s">
+      <c r="A131" s="69" t="s">
         <v>130</v>
       </c>
       <c r="B131">
@@ -2858,7 +2914,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="41" t="s">
+      <c r="A132" s="69" t="s">
         <v>131</v>
       </c>
       <c r="B132">
@@ -2869,7 +2925,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="41" t="s">
+      <c r="A133" s="69" t="s">
         <v>132</v>
       </c>
       <c r="B133">
@@ -2880,7 +2936,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="41" t="s">
+      <c r="A134" s="69" t="s">
         <v>133</v>
       </c>
       <c r="B134">
@@ -2891,7 +2947,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="41" t="s">
+      <c r="A135" s="69" t="s">
         <v>134</v>
       </c>
       <c r="B135">
@@ -2902,7 +2958,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="41" t="s">
+      <c r="A136" s="69" t="s">
         <v>135</v>
       </c>
       <c r="B136">
@@ -2913,7 +2969,7 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="41" t="s">
+      <c r="A137" s="69" t="s">
         <v>136</v>
       </c>
       <c r="B137">
@@ -2924,7 +2980,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="41" t="s">
+      <c r="A138" s="69" t="s">
         <v>137</v>
       </c>
       <c r="B138">
@@ -2935,7 +2991,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="41" t="s">
+      <c r="A139" s="69" t="s">
         <v>138</v>
       </c>
       <c r="B139">
@@ -2946,7 +3002,7 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="41" t="s">
+      <c r="A140" s="69" t="s">
         <v>139</v>
       </c>
       <c r="B140">
@@ -2957,7 +3013,7 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="41" t="s">
+      <c r="A141" s="69" t="s">
         <v>140</v>
       </c>
       <c r="B141">
@@ -2968,7 +3024,7 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="41" t="s">
+      <c r="A142" s="69" t="s">
         <v>141</v>
       </c>
       <c r="B142">
@@ -2979,7 +3035,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="41" t="s">
+      <c r="A143" s="69" t="s">
         <v>142</v>
       </c>
       <c r="B143">
@@ -2990,7 +3046,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="41" t="s">
+      <c r="A144" s="69" t="s">
         <v>143</v>
       </c>
       <c r="B144">
@@ -3001,7 +3057,7 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="41" t="s">
+      <c r="A145" s="69" t="s">
         <v>144</v>
       </c>
       <c r="B145">
@@ -3012,7 +3068,7 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="41" t="s">
+      <c r="A146" s="69" t="s">
         <v>145</v>
       </c>
       <c r="B146">
@@ -3023,7 +3079,7 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="41" t="s">
+      <c r="A147" s="69" t="s">
         <v>146</v>
       </c>
       <c r="B147">
@@ -3034,7 +3090,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="41" t="s">
+      <c r="A148" s="69" t="s">
         <v>147</v>
       </c>
       <c r="B148">
@@ -3045,7 +3101,7 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="41" t="s">
+      <c r="A149" s="69" t="s">
         <v>148</v>
       </c>
       <c r="B149">
@@ -3056,7 +3112,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="41" t="s">
+      <c r="A150" s="69" t="s">
         <v>149</v>
       </c>
       <c r="B150">
@@ -3067,7 +3123,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="41" t="s">
+      <c r="A151" s="69" t="s">
         <v>150</v>
       </c>
       <c r="B151">
@@ -3078,7 +3134,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="41" t="s">
+      <c r="A152" s="69" t="s">
         <v>151</v>
       </c>
       <c r="B152">
@@ -3089,7 +3145,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="41" t="s">
+      <c r="A153" s="69" t="s">
         <v>152</v>
       </c>
       <c r="B153">
@@ -3100,7 +3156,7 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="41" t="s">
+      <c r="A154" s="69" t="s">
         <v>153</v>
       </c>
       <c r="B154">
@@ -3111,7 +3167,7 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="41" t="s">
+      <c r="A155" s="69" t="s">
         <v>154</v>
       </c>
       <c r="B155">
@@ -3122,7 +3178,7 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="41" t="s">
+      <c r="A156" s="69" t="s">
         <v>155</v>
       </c>
       <c r="B156">
@@ -3133,7 +3189,7 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="41" t="s">
+      <c r="A157" s="69" t="s">
         <v>156</v>
       </c>
       <c r="B157">
@@ -3144,7 +3200,7 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="41" t="s">
+      <c r="A158" s="69" t="s">
         <v>157</v>
       </c>
       <c r="B158">
@@ -3155,7 +3211,7 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="41" t="s">
+      <c r="A159" s="69" t="s">
         <v>158</v>
       </c>
       <c r="B159">
@@ -3166,7 +3222,7 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="41" t="s">
+      <c r="A160" s="69" t="s">
         <v>159</v>
       </c>
       <c r="B160">
@@ -3177,7 +3233,7 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="41" t="s">
+      <c r="A161" s="69" t="s">
         <v>160</v>
       </c>
       <c r="B161">
@@ -3188,7 +3244,7 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="41" t="s">
+      <c r="A162" s="69" t="s">
         <v>161</v>
       </c>
       <c r="B162">
@@ -3199,7 +3255,7 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="41" t="s">
+      <c r="A163" s="69" t="s">
         <v>162</v>
       </c>
       <c r="B163">
@@ -3210,7 +3266,7 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="41" t="s">
+      <c r="A164" s="69" t="s">
         <v>163</v>
       </c>
       <c r="B164">
@@ -3221,7 +3277,7 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="41" t="s">
+      <c r="A165" s="69" t="s">
         <v>164</v>
       </c>
       <c r="B165">
@@ -3232,7 +3288,7 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" s="41" t="s">
+      <c r="A166" s="69" t="s">
         <v>165</v>
       </c>
       <c r="B166">
@@ -3243,7 +3299,7 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="41" t="s">
+      <c r="A167" s="69" t="s">
         <v>166</v>
       </c>
       <c r="B167">
@@ -3254,7 +3310,7 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="41" t="s">
+      <c r="A168" s="69" t="s">
         <v>167</v>
       </c>
       <c r="B168">
@@ -3265,7 +3321,7 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="41" t="s">
+      <c r="A169" s="69" t="s">
         <v>168</v>
       </c>
       <c r="B169">
@@ -3276,7 +3332,7 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="41" t="s">
+      <c r="A170" s="69" t="s">
         <v>169</v>
       </c>
       <c r="B170">
@@ -3287,7 +3343,7 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="41" t="s">
+      <c r="A171" s="69" t="s">
         <v>170</v>
       </c>
       <c r="B171">
@@ -3298,7 +3354,7 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="41" t="s">
+      <c r="A172" s="69" t="s">
         <v>171</v>
       </c>
       <c r="B172">
@@ -3309,7 +3365,7 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="41" t="s">
+      <c r="A173" s="69" t="s">
         <v>172</v>
       </c>
       <c r="B173">
@@ -3320,7 +3376,7 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="41" t="s">
+      <c r="A174" s="69" t="s">
         <v>173</v>
       </c>
       <c r="B174">
@@ -3331,7 +3387,7 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" s="41" t="s">
+      <c r="A175" s="69" t="s">
         <v>174</v>
       </c>
       <c r="B175">
@@ -3342,7 +3398,7 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="41" t="s">
+      <c r="A176" s="69" t="s">
         <v>175</v>
       </c>
       <c r="B176">
@@ -3353,7 +3409,7 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="41" t="s">
+      <c r="A177" s="69" t="s">
         <v>176</v>
       </c>
       <c r="B177">
@@ -3364,7 +3420,7 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="41" t="s">
+      <c r="A178" s="69" t="s">
         <v>177</v>
       </c>
       <c r="B178">
@@ -3375,7 +3431,7 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" s="41" t="s">
+      <c r="A179" s="69" t="s">
         <v>178</v>
       </c>
       <c r="B179">
@@ -3386,7 +3442,7 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="41" t="s">
+      <c r="A180" s="69" t="s">
         <v>179</v>
       </c>
       <c r="B180">
@@ -3397,7 +3453,7 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" s="41" t="s">
+      <c r="A181" s="69" t="s">
         <v>180</v>
       </c>
       <c r="B181">
@@ -3408,7 +3464,7 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" s="41" t="s">
+      <c r="A182" s="69" t="s">
         <v>181</v>
       </c>
       <c r="B182">
@@ -3419,7 +3475,7 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" s="41" t="s">
+      <c r="A183" s="69" t="s">
         <v>182</v>
       </c>
       <c r="B183">
@@ -3430,7 +3486,7 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="41" t="s">
+      <c r="A184" s="69" t="s">
         <v>183</v>
       </c>
       <c r="B184">
@@ -3441,7 +3497,7 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" s="41" t="s">
+      <c r="A185" s="69" t="s">
         <v>184</v>
       </c>
       <c r="B185">
@@ -3452,7 +3508,7 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" s="41" t="s">
+      <c r="A186" s="69" t="s">
         <v>185</v>
       </c>
       <c r="B186">
@@ -3463,7 +3519,7 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" s="41" t="s">
+      <c r="A187" s="69" t="s">
         <v>186</v>
       </c>
       <c r="B187">
@@ -3474,7 +3530,7 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" s="41" t="s">
+      <c r="A188" s="69" t="s">
         <v>187</v>
       </c>
       <c r="B188">
@@ -3485,7 +3541,7 @@
       </c>
     </row>
     <row r="189">
-      <c r="A189" s="41" t="s">
+      <c r="A189" s="69" t="s">
         <v>188</v>
       </c>
       <c r="B189">
@@ -3496,7 +3552,7 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" s="41" t="s">
+      <c r="A190" s="69" t="s">
         <v>189</v>
       </c>
       <c r="B190">
@@ -3507,7 +3563,7 @@
       </c>
     </row>
     <row r="191">
-      <c r="A191" s="41" t="s">
+      <c r="A191" s="69" t="s">
         <v>190</v>
       </c>
       <c r="B191">
@@ -3518,7 +3574,7 @@
       </c>
     </row>
     <row r="192">
-      <c r="A192" s="41" t="s">
+      <c r="A192" s="69" t="s">
         <v>191</v>
       </c>
       <c r="B192">
@@ -3529,7 +3585,7 @@
       </c>
     </row>
     <row r="193">
-      <c r="A193" s="41" t="s">
+      <c r="A193" s="69" t="s">
         <v>192</v>
       </c>
       <c r="B193">
@@ -3540,7 +3596,7 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" s="41" t="s">
+      <c r="A194" s="69" t="s">
         <v>193</v>
       </c>
       <c r="B194">
@@ -3551,7 +3607,7 @@
       </c>
     </row>
     <row r="195">
-      <c r="A195" s="41" t="s">
+      <c r="A195" s="69" t="s">
         <v>194</v>
       </c>
       <c r="B195">
@@ -3562,7 +3618,7 @@
       </c>
     </row>
     <row r="196">
-      <c r="A196" s="41" t="s">
+      <c r="A196" s="69" t="s">
         <v>195</v>
       </c>
       <c r="B196">
@@ -3573,7 +3629,7 @@
       </c>
     </row>
     <row r="197">
-      <c r="A197" s="41" t="s">
+      <c r="A197" s="69" t="s">
         <v>196</v>
       </c>
       <c r="B197">
@@ -3584,7 +3640,7 @@
       </c>
     </row>
     <row r="198">
-      <c r="A198" s="41" t="s">
+      <c r="A198" s="69" t="s">
         <v>197</v>
       </c>
       <c r="B198">
@@ -3595,7 +3651,7 @@
       </c>
     </row>
     <row r="199">
-      <c r="A199" s="41" t="s">
+      <c r="A199" s="69" t="s">
         <v>198</v>
       </c>
       <c r="B199">
@@ -3606,7 +3662,7 @@
       </c>
     </row>
     <row r="200">
-      <c r="A200" s="41" t="s">
+      <c r="A200" s="69" t="s">
         <v>199</v>
       </c>
       <c r="B200">
@@ -3617,7 +3673,7 @@
       </c>
     </row>
     <row r="201">
-      <c r="A201" s="41" t="s">
+      <c r="A201" s="69" t="s">
         <v>200</v>
       </c>
       <c r="B201">
@@ -3628,7 +3684,7 @@
       </c>
     </row>
     <row r="202">
-      <c r="A202" s="41" t="s">
+      <c r="A202" s="69" t="s">
         <v>201</v>
       </c>
       <c r="B202">
@@ -3639,7 +3695,7 @@
       </c>
     </row>
     <row r="203">
-      <c r="A203" s="41" t="s">
+      <c r="A203" s="69" t="s">
         <v>202</v>
       </c>
       <c r="B203">
@@ -3650,7 +3706,7 @@
       </c>
     </row>
     <row r="204">
-      <c r="A204" s="41" t="s">
+      <c r="A204" s="69" t="s">
         <v>203</v>
       </c>
       <c r="B204">
@@ -3661,7 +3717,7 @@
       </c>
     </row>
     <row r="205">
-      <c r="A205" s="41" t="s">
+      <c r="A205" s="69" t="s">
         <v>204</v>
       </c>
       <c r="B205">
@@ -3672,7 +3728,7 @@
       </c>
     </row>
     <row r="206">
-      <c r="A206" s="41" t="s">
+      <c r="A206" s="69" t="s">
         <v>205</v>
       </c>
       <c r="B206">
@@ -3683,7 +3739,7 @@
       </c>
     </row>
     <row r="207">
-      <c r="A207" s="41" t="s">
+      <c r="A207" s="69" t="s">
         <v>206</v>
       </c>
       <c r="B207">
@@ -3694,7 +3750,7 @@
       </c>
     </row>
     <row r="208">
-      <c r="A208" s="41" t="s">
+      <c r="A208" s="69" t="s">
         <v>207</v>
       </c>
       <c r="B208">
@@ -3705,7 +3761,7 @@
       </c>
     </row>
     <row r="209">
-      <c r="A209" s="41" t="s">
+      <c r="A209" s="69" t="s">
         <v>208</v>
       </c>
       <c r="B209">
@@ -3716,7 +3772,7 @@
       </c>
     </row>
     <row r="210">
-      <c r="A210" s="41" t="s">
+      <c r="A210" s="69" t="s">
         <v>209</v>
       </c>
       <c r="B210">
@@ -3727,7 +3783,7 @@
       </c>
     </row>
     <row r="211">
-      <c r="A211" s="41" t="s">
+      <c r="A211" s="69" t="s">
         <v>210</v>
       </c>
       <c r="B211">
@@ -3738,7 +3794,7 @@
       </c>
     </row>
     <row r="212">
-      <c r="A212" s="41" t="s">
+      <c r="A212" s="69" t="s">
         <v>211</v>
       </c>
       <c r="B212">
@@ -3749,7 +3805,7 @@
       </c>
     </row>
     <row r="213">
-      <c r="A213" s="41" t="s">
+      <c r="A213" s="69" t="s">
         <v>212</v>
       </c>
       <c r="B213">
@@ -3760,7 +3816,7 @@
       </c>
     </row>
     <row r="214">
-      <c r="A214" s="41" t="s">
+      <c r="A214" s="69" t="s">
         <v>213</v>
       </c>
       <c r="B214">
@@ -3771,7 +3827,7 @@
       </c>
     </row>
     <row r="215">
-      <c r="A215" s="41" t="s">
+      <c r="A215" s="69" t="s">
         <v>214</v>
       </c>
       <c r="B215">
@@ -3782,7 +3838,7 @@
       </c>
     </row>
     <row r="216">
-      <c r="A216" s="41" t="s">
+      <c r="A216" s="69" t="s">
         <v>215</v>
       </c>
       <c r="B216">
@@ -3793,7 +3849,7 @@
       </c>
     </row>
     <row r="217">
-      <c r="A217" s="41" t="s">
+      <c r="A217" s="69" t="s">
         <v>216</v>
       </c>
       <c r="B217">
@@ -3804,7 +3860,7 @@
       </c>
     </row>
     <row r="218">
-      <c r="A218" s="41" t="s">
+      <c r="A218" s="69" t="s">
         <v>217</v>
       </c>
       <c r="B218">
@@ -3815,7 +3871,7 @@
       </c>
     </row>
     <row r="219">
-      <c r="A219" s="41" t="s">
+      <c r="A219" s="69" t="s">
         <v>218</v>
       </c>
       <c r="B219">
@@ -3826,7 +3882,7 @@
       </c>
     </row>
     <row r="220">
-      <c r="A220" s="41" t="s">
+      <c r="A220" s="69" t="s">
         <v>219</v>
       </c>
       <c r="B220">
@@ -3837,7 +3893,7 @@
       </c>
     </row>
     <row r="221">
-      <c r="A221" s="41" t="s">
+      <c r="A221" s="69" t="s">
         <v>220</v>
       </c>
       <c r="B221">
@@ -3848,7 +3904,7 @@
       </c>
     </row>
     <row r="222">
-      <c r="A222" s="41" t="s">
+      <c r="A222" s="69" t="s">
         <v>221</v>
       </c>
       <c r="B222">
@@ -3859,7 +3915,7 @@
       </c>
     </row>
     <row r="223">
-      <c r="A223" s="41" t="s">
+      <c r="A223" s="69" t="s">
         <v>222</v>
       </c>
       <c r="B223">
@@ -3870,7 +3926,7 @@
       </c>
     </row>
     <row r="224">
-      <c r="A224" s="41" t="s">
+      <c r="A224" s="69" t="s">
         <v>223</v>
       </c>
       <c r="B224">
@@ -3881,7 +3937,7 @@
       </c>
     </row>
     <row r="225">
-      <c r="A225" s="41" t="s">
+      <c r="A225" s="69" t="s">
         <v>224</v>
       </c>
       <c r="B225">
@@ -3892,7 +3948,7 @@
       </c>
     </row>
     <row r="226">
-      <c r="A226" s="41" t="s">
+      <c r="A226" s="69" t="s">
         <v>225</v>
       </c>
       <c r="B226">
@@ -3903,7 +3959,7 @@
       </c>
     </row>
     <row r="227">
-      <c r="A227" s="41" t="s">
+      <c r="A227" s="69" t="s">
         <v>226</v>
       </c>
       <c r="B227">
@@ -3914,7 +3970,7 @@
       </c>
     </row>
     <row r="228">
-      <c r="A228" s="41" t="s">
+      <c r="A228" s="69" t="s">
         <v>227</v>
       </c>
       <c r="B228">
@@ -3925,7 +3981,7 @@
       </c>
     </row>
     <row r="229">
-      <c r="A229" s="41" t="s">
+      <c r="A229" s="69" t="s">
         <v>228</v>
       </c>
       <c r="B229">
@@ -3936,7 +3992,7 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" s="41" t="s">
+      <c r="A230" s="69" t="s">
         <v>229</v>
       </c>
       <c r="B230">
@@ -3947,7 +4003,7 @@
       </c>
     </row>
     <row r="231">
-      <c r="A231" s="41" t="s">
+      <c r="A231" s="69" t="s">
         <v>230</v>
       </c>
       <c r="B231">
@@ -3958,7 +4014,7 @@
       </c>
     </row>
     <row r="232">
-      <c r="A232" s="41" t="s">
+      <c r="A232" s="69" t="s">
         <v>231</v>
       </c>
       <c r="B232">
@@ -3969,7 +4025,7 @@
       </c>
     </row>
     <row r="233">
-      <c r="A233" s="41" t="s">
+      <c r="A233" s="69" t="s">
         <v>232</v>
       </c>
       <c r="B233">
@@ -3980,7 +4036,7 @@
       </c>
     </row>
     <row r="234">
-      <c r="A234" s="41" t="s">
+      <c r="A234" s="69" t="s">
         <v>233</v>
       </c>
       <c r="B234">
@@ -3991,7 +4047,7 @@
       </c>
     </row>
     <row r="235">
-      <c r="A235" s="41" t="s">
+      <c r="A235" s="69" t="s">
         <v>234</v>
       </c>
       <c r="B235">
@@ -4002,7 +4058,7 @@
       </c>
     </row>
     <row r="236">
-      <c r="A236" s="41" t="s">
+      <c r="A236" s="69" t="s">
         <v>235</v>
       </c>
       <c r="B236">
@@ -4013,7 +4069,7 @@
       </c>
     </row>
     <row r="237">
-      <c r="A237" s="41" t="s">
+      <c r="A237" s="69" t="s">
         <v>236</v>
       </c>
       <c r="B237">
@@ -4024,7 +4080,7 @@
       </c>
     </row>
     <row r="238">
-      <c r="A238" s="41" t="s">
+      <c r="A238" s="69" t="s">
         <v>237</v>
       </c>
       <c r="B238">
@@ -4035,7 +4091,7 @@
       </c>
     </row>
     <row r="239">
-      <c r="A239" s="41" t="s">
+      <c r="A239" s="69" t="s">
         <v>238</v>
       </c>
       <c r="B239">
@@ -4046,7 +4102,7 @@
       </c>
     </row>
     <row r="240">
-      <c r="A240" s="41" t="s">
+      <c r="A240" s="69" t="s">
         <v>239</v>
       </c>
       <c r="B240">
@@ -4057,7 +4113,7 @@
       </c>
     </row>
     <row r="241">
-      <c r="A241" s="41" t="s">
+      <c r="A241" s="69" t="s">
         <v>240</v>
       </c>
       <c r="B241">
@@ -4068,7 +4124,7 @@
       </c>
     </row>
     <row r="242">
-      <c r="A242" s="41" t="s">
+      <c r="A242" s="69" t="s">
         <v>241</v>
       </c>
       <c r="B242">
@@ -4079,7 +4135,7 @@
       </c>
     </row>
     <row r="243">
-      <c r="A243" s="41" t="s">
+      <c r="A243" s="69" t="s">
         <v>242</v>
       </c>
       <c r="B243">
@@ -4090,7 +4146,7 @@
       </c>
     </row>
     <row r="244">
-      <c r="A244" s="41" t="s">
+      <c r="A244" s="69" t="s">
         <v>243</v>
       </c>
       <c r="B244">
@@ -4101,7 +4157,7 @@
       </c>
     </row>
     <row r="245">
-      <c r="A245" s="41" t="s">
+      <c r="A245" s="69" t="s">
         <v>244</v>
       </c>
       <c r="B245">
@@ -4112,7 +4168,7 @@
       </c>
     </row>
     <row r="246">
-      <c r="A246" s="41" t="s">
+      <c r="A246" s="69" t="s">
         <v>245</v>
       </c>
       <c r="B246">
@@ -4123,7 +4179,7 @@
       </c>
     </row>
     <row r="247">
-      <c r="A247" s="41" t="s">
+      <c r="A247" s="69" t="s">
         <v>246</v>
       </c>
       <c r="B247">
@@ -4134,7 +4190,7 @@
       </c>
     </row>
     <row r="248">
-      <c r="A248" s="41" t="s">
+      <c r="A248" s="69" t="s">
         <v>247</v>
       </c>
       <c r="B248">
@@ -4145,7 +4201,7 @@
       </c>
     </row>
     <row r="249">
-      <c r="A249" s="41" t="s">
+      <c r="A249" s="69" t="s">
         <v>248</v>
       </c>
       <c r="B249">
@@ -4156,7 +4212,7 @@
       </c>
     </row>
     <row r="250">
-      <c r="A250" s="41" t="s">
+      <c r="A250" s="69" t="s">
         <v>249</v>
       </c>
       <c r="B250">
@@ -4167,7 +4223,7 @@
       </c>
     </row>
     <row r="251">
-      <c r="A251" s="41" t="s">
+      <c r="A251" s="69" t="s">
         <v>250</v>
       </c>
       <c r="B251">
@@ -4178,7 +4234,7 @@
       </c>
     </row>
     <row r="252">
-      <c r="A252" s="41" t="s">
+      <c r="A252" s="69" t="s">
         <v>251</v>
       </c>
       <c r="B252">
@@ -4189,7 +4245,7 @@
       </c>
     </row>
     <row r="253">
-      <c r="A253" s="41" t="s">
+      <c r="A253" s="69" t="s">
         <v>252</v>
       </c>
       <c r="B253">
@@ -4200,7 +4256,7 @@
       </c>
     </row>
     <row r="254">
-      <c r="A254" s="41" t="s">
+      <c r="A254" s="69" t="s">
         <v>253</v>
       </c>
       <c r="B254">
@@ -4211,7 +4267,7 @@
       </c>
     </row>
     <row r="255">
-      <c r="A255" s="41" t="s">
+      <c r="A255" s="69" t="s">
         <v>254</v>
       </c>
       <c r="B255">
@@ -4222,7 +4278,7 @@
       </c>
     </row>
     <row r="256">
-      <c r="A256" s="41" t="s">
+      <c r="A256" s="69" t="s">
         <v>255</v>
       </c>
       <c r="B256">
@@ -4233,7 +4289,7 @@
       </c>
     </row>
     <row r="257">
-      <c r="A257" s="41" t="s">
+      <c r="A257" s="69" t="s">
         <v>256</v>
       </c>
       <c r="B257">
@@ -4244,7 +4300,7 @@
       </c>
     </row>
     <row r="258">
-      <c r="A258" s="41" t="s">
+      <c r="A258" s="69" t="s">
         <v>257</v>
       </c>
       <c r="B258">
@@ -4255,7 +4311,7 @@
       </c>
     </row>
     <row r="259">
-      <c r="A259" s="41" t="s">
+      <c r="A259" s="69" t="s">
         <v>258</v>
       </c>
       <c r="B259">
@@ -4266,7 +4322,7 @@
       </c>
     </row>
     <row r="260">
-      <c r="A260" s="41" t="s">
+      <c r="A260" s="69" t="s">
         <v>259</v>
       </c>
       <c r="B260">
@@ -4277,7 +4333,7 @@
       </c>
     </row>
     <row r="261">
-      <c r="A261" s="41" t="s">
+      <c r="A261" s="69" t="s">
         <v>260</v>
       </c>
       <c r="B261">
@@ -4288,7 +4344,7 @@
       </c>
     </row>
     <row r="262">
-      <c r="A262" s="41" t="s">
+      <c r="A262" s="69" t="s">
         <v>261</v>
       </c>
       <c r="B262">
@@ -4299,7 +4355,7 @@
       </c>
     </row>
     <row r="263">
-      <c r="A263" s="41" t="s">
+      <c r="A263" s="69" t="s">
         <v>262</v>
       </c>
       <c r="B263">
@@ -4310,7 +4366,7 @@
       </c>
     </row>
     <row r="264">
-      <c r="A264" s="41" t="s">
+      <c r="A264" s="69" t="s">
         <v>263</v>
       </c>
       <c r="B264">
@@ -4321,7 +4377,7 @@
       </c>
     </row>
     <row r="265">
-      <c r="A265" s="41" t="s">
+      <c r="A265" s="69" t="s">
         <v>264</v>
       </c>
       <c r="B265">
@@ -4332,7 +4388,7 @@
       </c>
     </row>
     <row r="266">
-      <c r="A266" s="41" t="s">
+      <c r="A266" s="69" t="s">
         <v>265</v>
       </c>
       <c r="B266">
@@ -4343,7 +4399,7 @@
       </c>
     </row>
     <row r="267">
-      <c r="A267" s="41" t="s">
+      <c r="A267" s="69" t="s">
         <v>266</v>
       </c>
       <c r="B267">
@@ -4354,7 +4410,7 @@
       </c>
     </row>
     <row r="268">
-      <c r="A268" s="41" t="s">
+      <c r="A268" s="69" t="s">
         <v>267</v>
       </c>
       <c r="B268">
@@ -4365,7 +4421,7 @@
       </c>
     </row>
     <row r="269">
-      <c r="A269" s="41" t="s">
+      <c r="A269" s="69" t="s">
         <v>268</v>
       </c>
       <c r="B269">
@@ -4376,7 +4432,7 @@
       </c>
     </row>
     <row r="270">
-      <c r="A270" s="41" t="s">
+      <c r="A270" s="69" t="s">
         <v>269</v>
       </c>
       <c r="B270">
@@ -4387,7 +4443,7 @@
       </c>
     </row>
     <row r="271">
-      <c r="A271" s="41" t="s">
+      <c r="A271" s="69" t="s">
         <v>270</v>
       </c>
       <c r="B271">
@@ -4398,7 +4454,7 @@
       </c>
     </row>
     <row r="272">
-      <c r="A272" s="41" t="s">
+      <c r="A272" s="69" t="s">
         <v>271</v>
       </c>
       <c r="B272">
@@ -4409,7 +4465,7 @@
       </c>
     </row>
     <row r="273">
-      <c r="A273" s="41" t="s">
+      <c r="A273" s="69" t="s">
         <v>272</v>
       </c>
       <c r="B273">
@@ -4420,7 +4476,7 @@
       </c>
     </row>
     <row r="274">
-      <c r="A274" s="41" t="s">
+      <c r="A274" s="69" t="s">
         <v>273</v>
       </c>
       <c r="B274">
@@ -4431,7 +4487,7 @@
       </c>
     </row>
     <row r="275">
-      <c r="A275" s="41" t="s">
+      <c r="A275" s="69" t="s">
         <v>274</v>
       </c>
       <c r="B275">
@@ -4442,7 +4498,7 @@
       </c>
     </row>
     <row r="276">
-      <c r="A276" s="41" t="s">
+      <c r="A276" s="69" t="s">
         <v>275</v>
       </c>
       <c r="B276">
@@ -4453,7 +4509,7 @@
       </c>
     </row>
     <row r="277">
-      <c r="A277" s="41" t="s">
+      <c r="A277" s="69" t="s">
         <v>276</v>
       </c>
       <c r="B277">
@@ -4464,7 +4520,7 @@
       </c>
     </row>
     <row r="278">
-      <c r="A278" s="41" t="s">
+      <c r="A278" s="69" t="s">
         <v>277</v>
       </c>
       <c r="B278">
@@ -4475,7 +4531,7 @@
       </c>
     </row>
     <row r="279">
-      <c r="A279" s="41" t="s">
+      <c r="A279" s="69" t="s">
         <v>278</v>
       </c>
       <c r="B279">
@@ -4486,7 +4542,7 @@
       </c>
     </row>
     <row r="280">
-      <c r="A280" s="41" t="s">
+      <c r="A280" s="69" t="s">
         <v>279</v>
       </c>
       <c r="B280">
@@ -4497,7 +4553,7 @@
       </c>
     </row>
     <row r="281">
-      <c r="A281" s="41" t="s">
+      <c r="A281" s="69" t="s">
         <v>280</v>
       </c>
       <c r="B281">
@@ -4508,7 +4564,7 @@
       </c>
     </row>
     <row r="282">
-      <c r="A282" s="41" t="s">
+      <c r="A282" s="69" t="s">
         <v>281</v>
       </c>
       <c r="B282">
@@ -4519,7 +4575,7 @@
       </c>
     </row>
     <row r="283">
-      <c r="A283" s="41" t="s">
+      <c r="A283" s="69" t="s">
         <v>282</v>
       </c>
       <c r="B283">
@@ -4530,7 +4586,7 @@
       </c>
     </row>
     <row r="284">
-      <c r="A284" s="41" t="s">
+      <c r="A284" s="69" t="s">
         <v>283</v>
       </c>
       <c r="B284">
@@ -4541,7 +4597,7 @@
       </c>
     </row>
     <row r="285">
-      <c r="A285" s="41" t="s">
+      <c r="A285" s="69" t="s">
         <v>284</v>
       </c>
       <c r="B285">
@@ -4552,7 +4608,7 @@
       </c>
     </row>
     <row r="286">
-      <c r="A286" s="41" t="s">
+      <c r="A286" s="69" t="s">
         <v>285</v>
       </c>
       <c r="B286">
@@ -4563,7 +4619,7 @@
       </c>
     </row>
     <row r="287">
-      <c r="A287" s="41" t="s">
+      <c r="A287" s="69" t="s">
         <v>286</v>
       </c>
       <c r="B287">
@@ -4574,7 +4630,7 @@
       </c>
     </row>
     <row r="288">
-      <c r="A288" s="41" t="s">
+      <c r="A288" s="69" t="s">
         <v>287</v>
       </c>
       <c r="B288">
@@ -4585,7 +4641,7 @@
       </c>
     </row>
     <row r="289">
-      <c r="A289" s="41" t="s">
+      <c r="A289" s="69" t="s">
         <v>288</v>
       </c>
       <c r="B289">
@@ -4596,7 +4652,7 @@
       </c>
     </row>
     <row r="290">
-      <c r="A290" s="41" t="s">
+      <c r="A290" s="69" t="s">
         <v>289</v>
       </c>
       <c r="B290">
@@ -4607,7 +4663,7 @@
       </c>
     </row>
     <row r="291">
-      <c r="A291" s="41" t="s">
+      <c r="A291" s="69" t="s">
         <v>290</v>
       </c>
       <c r="B291">
@@ -4618,7 +4674,7 @@
       </c>
     </row>
     <row r="292">
-      <c r="A292" s="41" t="s">
+      <c r="A292" s="69" t="s">
         <v>291</v>
       </c>
       <c r="B292">
@@ -4629,7 +4685,7 @@
       </c>
     </row>
     <row r="293">
-      <c r="A293" s="41" t="s">
+      <c r="A293" s="69" t="s">
         <v>292</v>
       </c>
       <c r="B293">
@@ -4640,7 +4696,7 @@
       </c>
     </row>
     <row r="294">
-      <c r="A294" s="41" t="s">
+      <c r="A294" s="69" t="s">
         <v>293</v>
       </c>
       <c r="B294">
@@ -4651,7 +4707,7 @@
       </c>
     </row>
     <row r="295">
-      <c r="A295" s="41" t="s">
+      <c r="A295" s="69" t="s">
         <v>294</v>
       </c>
       <c r="B295">
@@ -4662,7 +4718,7 @@
       </c>
     </row>
     <row r="296">
-      <c r="A296" s="41" t="s">
+      <c r="A296" s="69" t="s">
         <v>295</v>
       </c>
       <c r="B296">
@@ -4673,7 +4729,7 @@
       </c>
     </row>
     <row r="297">
-      <c r="A297" s="41" t="s">
+      <c r="A297" s="69" t="s">
         <v>296</v>
       </c>
       <c r="B297">
@@ -4684,7 +4740,7 @@
       </c>
     </row>
     <row r="298">
-      <c r="A298" s="41" t="s">
+      <c r="A298" s="69" t="s">
         <v>297</v>
       </c>
       <c r="B298">
@@ -4695,7 +4751,7 @@
       </c>
     </row>
     <row r="299">
-      <c r="A299" s="41" t="s">
+      <c r="A299" s="69" t="s">
         <v>298</v>
       </c>
       <c r="B299">
@@ -4706,7 +4762,7 @@
       </c>
     </row>
     <row r="300">
-      <c r="A300" s="41" t="s">
+      <c r="A300" s="69" t="s">
         <v>299</v>
       </c>
       <c r="B300">
@@ -4717,7 +4773,7 @@
       </c>
     </row>
     <row r="301">
-      <c r="A301" s="41" t="s">
+      <c r="A301" s="69" t="s">
         <v>300</v>
       </c>
       <c r="B301">
@@ -4728,7 +4784,7 @@
       </c>
     </row>
     <row r="302">
-      <c r="A302" s="41" t="s">
+      <c r="A302" s="69" t="s">
         <v>301</v>
       </c>
       <c r="B302">
@@ -4739,7 +4795,7 @@
       </c>
     </row>
     <row r="303">
-      <c r="A303" s="41" t="s">
+      <c r="A303" s="69" t="s">
         <v>302</v>
       </c>
       <c r="B303">
@@ -4750,7 +4806,7 @@
       </c>
     </row>
     <row r="304">
-      <c r="A304" s="41" t="s">
+      <c r="A304" s="69" t="s">
         <v>303</v>
       </c>
       <c r="B304">
@@ -4761,7 +4817,7 @@
       </c>
     </row>
     <row r="305">
-      <c r="A305" s="41" t="s">
+      <c r="A305" s="69" t="s">
         <v>304</v>
       </c>
       <c r="B305">
@@ -4772,7 +4828,7 @@
       </c>
     </row>
     <row r="306">
-      <c r="A306" s="41" t="s">
+      <c r="A306" s="69" t="s">
         <v>305</v>
       </c>
       <c r="B306">
@@ -4783,7 +4839,7 @@
       </c>
     </row>
     <row r="307">
-      <c r="A307" s="41" t="s">
+      <c r="A307" s="69" t="s">
         <v>306</v>
       </c>
       <c r="B307">
@@ -4794,7 +4850,7 @@
       </c>
     </row>
     <row r="308">
-      <c r="A308" s="41" t="s">
+      <c r="A308" s="69" t="s">
         <v>307</v>
       </c>
       <c r="B308">
@@ -4805,7 +4861,7 @@
       </c>
     </row>
     <row r="309">
-      <c r="A309" s="41" t="s">
+      <c r="A309" s="69" t="s">
         <v>308</v>
       </c>
       <c r="B309">
@@ -4816,7 +4872,7 @@
       </c>
     </row>
     <row r="310">
-      <c r="A310" s="41" t="s">
+      <c r="A310" s="69" t="s">
         <v>309</v>
       </c>
       <c r="B310">
@@ -4827,7 +4883,7 @@
       </c>
     </row>
     <row r="311">
-      <c r="A311" s="41" t="s">
+      <c r="A311" s="69" t="s">
         <v>310</v>
       </c>
       <c r="B311">
@@ -4838,7 +4894,7 @@
       </c>
     </row>
     <row r="312">
-      <c r="A312" s="41" t="s">
+      <c r="A312" s="69" t="s">
         <v>311</v>
       </c>
       <c r="B312">
@@ -4849,7 +4905,7 @@
       </c>
     </row>
     <row r="313">
-      <c r="A313" s="41" t="s">
+      <c r="A313" s="69" t="s">
         <v>312</v>
       </c>
       <c r="B313">
@@ -4860,7 +4916,7 @@
       </c>
     </row>
     <row r="314">
-      <c r="A314" s="41" t="s">
+      <c r="A314" s="69" t="s">
         <v>313</v>
       </c>
       <c r="B314">
@@ -4871,7 +4927,7 @@
       </c>
     </row>
     <row r="315">
-      <c r="A315" s="41" t="s">
+      <c r="A315" s="69" t="s">
         <v>314</v>
       </c>
       <c r="B315">
@@ -4882,7 +4938,7 @@
       </c>
     </row>
     <row r="316">
-      <c r="A316" s="41" t="s">
+      <c r="A316" s="69" t="s">
         <v>315</v>
       </c>
       <c r="B316">
@@ -4893,7 +4949,7 @@
       </c>
     </row>
     <row r="317">
-      <c r="A317" s="41" t="s">
+      <c r="A317" s="69" t="s">
         <v>316</v>
       </c>
       <c r="B317">
@@ -4904,7 +4960,7 @@
       </c>
     </row>
     <row r="318">
-      <c r="A318" s="41" t="s">
+      <c r="A318" s="69" t="s">
         <v>317</v>
       </c>
       <c r="B318">
@@ -4915,7 +4971,7 @@
       </c>
     </row>
     <row r="319">
-      <c r="A319" s="41" t="s">
+      <c r="A319" s="69" t="s">
         <v>318</v>
       </c>
       <c r="B319">
@@ -4926,7 +4982,7 @@
       </c>
     </row>
     <row r="320">
-      <c r="A320" s="41" t="s">
+      <c r="A320" s="69" t="s">
         <v>319</v>
       </c>
       <c r="B320">
@@ -4937,7 +4993,7 @@
       </c>
     </row>
     <row r="321">
-      <c r="A321" s="41" t="s">
+      <c r="A321" s="69" t="s">
         <v>320</v>
       </c>
       <c r="B321">
@@ -4948,7 +5004,7 @@
       </c>
     </row>
     <row r="322">
-      <c r="A322" s="41" t="s">
+      <c r="A322" s="69" t="s">
         <v>321</v>
       </c>
       <c r="B322">
@@ -4959,7 +5015,7 @@
       </c>
     </row>
     <row r="323">
-      <c r="A323" s="41" t="s">
+      <c r="A323" s="69" t="s">
         <v>322</v>
       </c>
       <c r="B323">
@@ -4970,7 +5026,7 @@
       </c>
     </row>
     <row r="324">
-      <c r="A324" s="41" t="s">
+      <c r="A324" s="69" t="s">
         <v>323</v>
       </c>
       <c r="B324">
@@ -4981,7 +5037,7 @@
       </c>
     </row>
     <row r="325">
-      <c r="A325" s="41" t="s">
+      <c r="A325" s="69" t="s">
         <v>324</v>
       </c>
       <c r="B325">
@@ -4992,7 +5048,7 @@
       </c>
     </row>
     <row r="326">
-      <c r="A326" s="41" t="s">
+      <c r="A326" s="69" t="s">
         <v>325</v>
       </c>
       <c r="B326">
@@ -5003,7 +5059,7 @@
       </c>
     </row>
     <row r="327">
-      <c r="A327" s="41" t="s">
+      <c r="A327" s="69" t="s">
         <v>326</v>
       </c>
       <c r="B327">
@@ -5014,7 +5070,7 @@
       </c>
     </row>
     <row r="328">
-      <c r="A328" s="41" t="s">
+      <c r="A328" s="69" t="s">
         <v>327</v>
       </c>
       <c r="B328">
@@ -5025,7 +5081,7 @@
       </c>
     </row>
     <row r="329">
-      <c r="A329" s="41" t="s">
+      <c r="A329" s="69" t="s">
         <v>328</v>
       </c>
       <c r="B329">
@@ -5036,7 +5092,7 @@
       </c>
     </row>
     <row r="330">
-      <c r="A330" s="41" t="s">
+      <c r="A330" s="69" t="s">
         <v>329</v>
       </c>
       <c r="B330">
@@ -5047,7 +5103,7 @@
       </c>
     </row>
     <row r="331">
-      <c r="A331" s="41" t="s">
+      <c r="A331" s="69" t="s">
         <v>330</v>
       </c>
       <c r="B331">
@@ -5058,7 +5114,7 @@
       </c>
     </row>
     <row r="332">
-      <c r="A332" s="41" t="s">
+      <c r="A332" s="69" t="s">
         <v>331</v>
       </c>
       <c r="B332">
@@ -5069,7 +5125,7 @@
       </c>
     </row>
     <row r="333">
-      <c r="A333" s="41" t="s">
+      <c r="A333" s="69" t="s">
         <v>332</v>
       </c>
       <c r="B333">
@@ -5080,7 +5136,7 @@
       </c>
     </row>
     <row r="334">
-      <c r="A334" s="41" t="s">
+      <c r="A334" s="69" t="s">
         <v>333</v>
       </c>
       <c r="B334">
@@ -5091,7 +5147,7 @@
       </c>
     </row>
     <row r="335">
-      <c r="A335" s="41" t="s">
+      <c r="A335" s="69" t="s">
         <v>334</v>
       </c>
       <c r="B335">
@@ -5102,7 +5158,7 @@
       </c>
     </row>
     <row r="336">
-      <c r="A336" s="41" t="s">
+      <c r="A336" s="69" t="s">
         <v>335</v>
       </c>
       <c r="B336">
@@ -5113,7 +5169,7 @@
       </c>
     </row>
     <row r="337">
-      <c r="A337" s="41" t="s">
+      <c r="A337" s="69" t="s">
         <v>336</v>
       </c>
       <c r="B337">
@@ -5124,7 +5180,7 @@
       </c>
     </row>
     <row r="338">
-      <c r="A338" s="41" t="s">
+      <c r="A338" s="69" t="s">
         <v>337</v>
       </c>
       <c r="B338">
@@ -5135,7 +5191,7 @@
       </c>
     </row>
     <row r="339">
-      <c r="A339" s="41" t="s">
+      <c r="A339" s="69" t="s">
         <v>338</v>
       </c>
       <c r="B339">
@@ -5146,7 +5202,7 @@
       </c>
     </row>
     <row r="340">
-      <c r="A340" s="41" t="s">
+      <c r="A340" s="69" t="s">
         <v>339</v>
       </c>
       <c r="B340">
@@ -5157,7 +5213,7 @@
       </c>
     </row>
     <row r="341">
-      <c r="A341" s="41" t="s">
+      <c r="A341" s="69" t="s">
         <v>340</v>
       </c>
       <c r="B341">
@@ -5168,7 +5224,7 @@
       </c>
     </row>
     <row r="342">
-      <c r="A342" s="41" t="s">
+      <c r="A342" s="69" t="s">
         <v>341</v>
       </c>
       <c r="B342">
@@ -5179,7 +5235,7 @@
       </c>
     </row>
     <row r="343">
-      <c r="A343" s="41" t="s">
+      <c r="A343" s="69" t="s">
         <v>342</v>
       </c>
       <c r="B343">
@@ -5190,7 +5246,7 @@
       </c>
     </row>
     <row r="344">
-      <c r="A344" s="41" t="s">
+      <c r="A344" s="69" t="s">
         <v>343</v>
       </c>
       <c r="B344">
@@ -5201,7 +5257,7 @@
       </c>
     </row>
     <row r="345">
-      <c r="A345" s="41" t="s">
+      <c r="A345" s="69" t="s">
         <v>344</v>
       </c>
       <c r="B345">
@@ -5212,7 +5268,7 @@
       </c>
     </row>
     <row r="346">
-      <c r="A346" s="41" t="s">
+      <c r="A346" s="69" t="s">
         <v>345</v>
       </c>
       <c r="B346">
@@ -5223,7 +5279,7 @@
       </c>
     </row>
     <row r="347">
-      <c r="A347" s="41" t="s">
+      <c r="A347" s="69" t="s">
         <v>346</v>
       </c>
       <c r="B347">
@@ -5234,7 +5290,7 @@
       </c>
     </row>
     <row r="348">
-      <c r="A348" s="41" t="s">
+      <c r="A348" s="69" t="s">
         <v>347</v>
       </c>
       <c r="B348">
@@ -5245,7 +5301,7 @@
       </c>
     </row>
     <row r="349">
-      <c r="A349" s="41" t="s">
+      <c r="A349" s="69" t="s">
         <v>348</v>
       </c>
       <c r="B349">
@@ -5256,7 +5312,7 @@
       </c>
     </row>
     <row r="350">
-      <c r="A350" s="41" t="s">
+      <c r="A350" s="69" t="s">
         <v>349</v>
       </c>
       <c r="B350">
@@ -5267,7 +5323,7 @@
       </c>
     </row>
     <row r="351">
-      <c r="A351" s="41" t="s">
+      <c r="A351" s="69" t="s">
         <v>350</v>
       </c>
       <c r="B351">
@@ -5278,7 +5334,7 @@
       </c>
     </row>
     <row r="352">
-      <c r="A352" s="41" t="s">
+      <c r="A352" s="69" t="s">
         <v>351</v>
       </c>
       <c r="B352">
@@ -5289,7 +5345,7 @@
       </c>
     </row>
     <row r="353">
-      <c r="A353" s="41" t="s">
+      <c r="A353" s="69" t="s">
         <v>352</v>
       </c>
       <c r="B353">
@@ -5300,7 +5356,7 @@
       </c>
     </row>
     <row r="354">
-      <c r="A354" s="41" t="s">
+      <c r="A354" s="69" t="s">
         <v>353</v>
       </c>
       <c r="B354">
@@ -5311,7 +5367,7 @@
       </c>
     </row>
     <row r="355">
-      <c r="A355" s="41" t="s">
+      <c r="A355" s="69" t="s">
         <v>354</v>
       </c>
       <c r="B355">
@@ -5322,7 +5378,7 @@
       </c>
     </row>
     <row r="356">
-      <c r="A356" s="41" t="s">
+      <c r="A356" s="69" t="s">
         <v>355</v>
       </c>
       <c r="B356">
@@ -5333,7 +5389,7 @@
       </c>
     </row>
     <row r="357">
-      <c r="A357" s="41" t="s">
+      <c r="A357" s="69" t="s">
         <v>356</v>
       </c>
       <c r="B357">
@@ -5344,7 +5400,7 @@
       </c>
     </row>
     <row r="358">
-      <c r="A358" s="41" t="s">
+      <c r="A358" s="69" t="s">
         <v>357</v>
       </c>
       <c r="B358">
@@ -5355,7 +5411,7 @@
       </c>
     </row>
     <row r="359">
-      <c r="A359" s="41" t="s">
+      <c r="A359" s="69" t="s">
         <v>358</v>
       </c>
       <c r="B359">
@@ -5366,7 +5422,7 @@
       </c>
     </row>
     <row r="360">
-      <c r="A360" s="41" t="s">
+      <c r="A360" s="69" t="s">
         <v>359</v>
       </c>
       <c r="B360">
@@ -5377,7 +5433,7 @@
       </c>
     </row>
     <row r="361">
-      <c r="A361" s="41" t="s">
+      <c r="A361" s="69" t="s">
         <v>360</v>
       </c>
       <c r="B361">
@@ -5388,7 +5444,7 @@
       </c>
     </row>
     <row r="362">
-      <c r="A362" s="41" t="s">
+      <c r="A362" s="69" t="s">
         <v>361</v>
       </c>
       <c r="B362">
@@ -5399,7 +5455,7 @@
       </c>
     </row>
     <row r="363">
-      <c r="A363" s="41" t="s">
+      <c r="A363" s="69" t="s">
         <v>362</v>
       </c>
       <c r="B363">
@@ -5410,7 +5466,7 @@
       </c>
     </row>
     <row r="364">
-      <c r="A364" s="41" t="s">
+      <c r="A364" s="69" t="s">
         <v>363</v>
       </c>
       <c r="B364">
@@ -5421,7 +5477,7 @@
       </c>
     </row>
     <row r="365">
-      <c r="A365" s="41" t="s">
+      <c r="A365" s="69" t="s">
         <v>364</v>
       </c>
       <c r="B365">
@@ -5432,7 +5488,7 @@
       </c>
     </row>
     <row r="366">
-      <c r="A366" s="41" t="s">
+      <c r="A366" s="69" t="s">
         <v>365</v>
       </c>
       <c r="B366">
@@ -5443,7 +5499,7 @@
       </c>
     </row>
     <row r="367">
-      <c r="A367" s="41" t="s">
+      <c r="A367" s="69" t="s">
         <v>366</v>
       </c>
       <c r="B367">
@@ -5454,7 +5510,7 @@
       </c>
     </row>
     <row r="368">
-      <c r="A368" s="41" t="s">
+      <c r="A368" s="69" t="s">
         <v>367</v>
       </c>
       <c r="B368">
@@ -5465,7 +5521,7 @@
       </c>
     </row>
     <row r="369">
-      <c r="A369" s="41" t="s">
+      <c r="A369" s="69" t="s">
         <v>368</v>
       </c>
       <c r="B369">
@@ -5476,7 +5532,7 @@
       </c>
     </row>
     <row r="370">
-      <c r="A370" s="41" t="s">
+      <c r="A370" s="69" t="s">
         <v>369</v>
       </c>
       <c r="B370">
@@ -5487,7 +5543,7 @@
       </c>
     </row>
     <row r="371">
-      <c r="A371" s="41" t="s">
+      <c r="A371" s="69" t="s">
         <v>370</v>
       </c>
       <c r="B371">
@@ -5498,7 +5554,7 @@
       </c>
     </row>
     <row r="372">
-      <c r="A372" s="41" t="s">
+      <c r="A372" s="69" t="s">
         <v>371</v>
       </c>
       <c r="B372">
@@ -5509,7 +5565,7 @@
       </c>
     </row>
     <row r="373">
-      <c r="A373" s="41" t="s">
+      <c r="A373" s="69" t="s">
         <v>372</v>
       </c>
       <c r="B373">
@@ -5520,7 +5576,7 @@
       </c>
     </row>
     <row r="374">
-      <c r="A374" s="41" t="s">
+      <c r="A374" s="69" t="s">
         <v>373</v>
       </c>
       <c r="B374">
@@ -5531,7 +5587,7 @@
       </c>
     </row>
     <row r="375">
-      <c r="A375" s="41" t="s">
+      <c r="A375" s="69" t="s">
         <v>374</v>
       </c>
       <c r="B375">
@@ -5542,7 +5598,7 @@
       </c>
     </row>
     <row r="376">
-      <c r="A376" s="41" t="s">
+      <c r="A376" s="69" t="s">
         <v>375</v>
       </c>
       <c r="B376">
@@ -5553,7 +5609,7 @@
       </c>
     </row>
     <row r="377">
-      <c r="A377" s="41" t="s">
+      <c r="A377" s="69" t="s">
         <v>376</v>
       </c>
       <c r="B377">
@@ -5564,7 +5620,7 @@
       </c>
     </row>
     <row r="378">
-      <c r="A378" s="41" t="s">
+      <c r="A378" s="69" t="s">
         <v>377</v>
       </c>
       <c r="B378">
@@ -5575,7 +5631,7 @@
       </c>
     </row>
     <row r="379">
-      <c r="A379" s="41" t="s">
+      <c r="A379" s="69" t="s">
         <v>378</v>
       </c>
       <c r="B379">
@@ -5586,7 +5642,7 @@
       </c>
     </row>
     <row r="380">
-      <c r="A380" s="41" t="s">
+      <c r="A380" s="69" t="s">
         <v>379</v>
       </c>
       <c r="B380">
@@ -5597,7 +5653,7 @@
       </c>
     </row>
     <row r="381">
-      <c r="A381" s="41" t="s">
+      <c r="A381" s="69" t="s">
         <v>380</v>
       </c>
       <c r="B381">
@@ -5608,7 +5664,7 @@
       </c>
     </row>
     <row r="382">
-      <c r="A382" s="41" t="s">
+      <c r="A382" s="69" t="s">
         <v>381</v>
       </c>
       <c r="B382">
@@ -5619,7 +5675,7 @@
       </c>
     </row>
     <row r="383">
-      <c r="A383" s="41" t="s">
+      <c r="A383" s="69" t="s">
         <v>382</v>
       </c>
       <c r="B383">
@@ -5630,7 +5686,7 @@
       </c>
     </row>
     <row r="384">
-      <c r="A384" s="41" t="s">
+      <c r="A384" s="69" t="s">
         <v>383</v>
       </c>
       <c r="B384">
@@ -5641,7 +5697,7 @@
       </c>
     </row>
     <row r="385">
-      <c r="A385" s="41" t="s">
+      <c r="A385" s="69" t="s">
         <v>384</v>
       </c>
       <c r="B385">
@@ -5652,7 +5708,7 @@
       </c>
     </row>
     <row r="386">
-      <c r="A386" s="41" t="s">
+      <c r="A386" s="69" t="s">
         <v>385</v>
       </c>
       <c r="B386">
@@ -5663,7 +5719,7 @@
       </c>
     </row>
     <row r="387">
-      <c r="A387" s="41" t="s">
+      <c r="A387" s="69" t="s">
         <v>386</v>
       </c>
       <c r="B387">
@@ -5674,7 +5730,7 @@
       </c>
     </row>
     <row r="388">
-      <c r="A388" s="41" t="s">
+      <c r="A388" s="69" t="s">
         <v>387</v>
       </c>
       <c r="B388">
@@ -5685,7 +5741,7 @@
       </c>
     </row>
     <row r="389">
-      <c r="A389" s="41" t="s">
+      <c r="A389" s="69" t="s">
         <v>388</v>
       </c>
       <c r="B389">
@@ -5696,7 +5752,7 @@
       </c>
     </row>
     <row r="390">
-      <c r="A390" s="41" t="s">
+      <c r="A390" s="69" t="s">
         <v>389</v>
       </c>
       <c r="B390">
@@ -5707,7 +5763,7 @@
       </c>
     </row>
     <row r="391">
-      <c r="A391" s="41" t="s">
+      <c r="A391" s="69" t="s">
         <v>390</v>
       </c>
       <c r="B391">
@@ -5718,7 +5774,7 @@
       </c>
     </row>
     <row r="392">
-      <c r="A392" s="41" t="s">
+      <c r="A392" s="69" t="s">
         <v>391</v>
       </c>
       <c r="B392">
@@ -5729,7 +5785,7 @@
       </c>
     </row>
     <row r="393">
-      <c r="A393" s="41" t="s">
+      <c r="A393" s="69" t="s">
         <v>392</v>
       </c>
       <c r="B393">
@@ -5740,7 +5796,7 @@
       </c>
     </row>
     <row r="394">
-      <c r="A394" s="41" t="s">
+      <c r="A394" s="69" t="s">
         <v>393</v>
       </c>
       <c r="B394">
@@ -5751,7 +5807,7 @@
       </c>
     </row>
     <row r="395">
-      <c r="A395" s="41" t="s">
+      <c r="A395" s="69" t="s">
         <v>394</v>
       </c>
       <c r="B395">
@@ -5762,7 +5818,7 @@
       </c>
     </row>
     <row r="396">
-      <c r="A396" s="41" t="s">
+      <c r="A396" s="69" t="s">
         <v>395</v>
       </c>
       <c r="B396">
@@ -5773,7 +5829,7 @@
       </c>
     </row>
     <row r="397">
-      <c r="A397" s="41" t="s">
+      <c r="A397" s="69" t="s">
         <v>396</v>
       </c>
       <c r="B397">
@@ -5784,7 +5840,7 @@
       </c>
     </row>
     <row r="398">
-      <c r="A398" s="41" t="s">
+      <c r="A398" s="69" t="s">
         <v>397</v>
       </c>
       <c r="B398">
@@ -5795,7 +5851,7 @@
       </c>
     </row>
     <row r="399">
-      <c r="A399" s="41" t="s">
+      <c r="A399" s="69" t="s">
         <v>398</v>
       </c>
       <c r="B399">
@@ -5806,7 +5862,7 @@
       </c>
     </row>
     <row r="400">
-      <c r="A400" s="41" t="s">
+      <c r="A400" s="69" t="s">
         <v>399</v>
       </c>
       <c r="B400">
@@ -5817,7 +5873,7 @@
       </c>
     </row>
     <row r="401">
-      <c r="A401" s="41" t="s">
+      <c r="A401" s="69" t="s">
         <v>400</v>
       </c>
       <c r="B401">
@@ -5828,7 +5884,7 @@
       </c>
     </row>
     <row r="402">
-      <c r="A402" s="41" t="s">
+      <c r="A402" s="69" t="s">
         <v>401</v>
       </c>
       <c r="B402">
@@ -5839,7 +5895,7 @@
       </c>
     </row>
     <row r="403">
-      <c r="A403" s="41" t="s">
+      <c r="A403" s="69" t="s">
         <v>402</v>
       </c>
       <c r="B403">
@@ -5850,7 +5906,7 @@
       </c>
     </row>
     <row r="404">
-      <c r="A404" s="41" t="s">
+      <c r="A404" s="69" t="s">
         <v>403</v>
       </c>
       <c r="B404">
@@ -5861,7 +5917,7 @@
       </c>
     </row>
     <row r="405">
-      <c r="A405" s="41" t="s">
+      <c r="A405" s="69" t="s">
         <v>404</v>
       </c>
       <c r="B405">
@@ -5872,7 +5928,7 @@
       </c>
     </row>
     <row r="406">
-      <c r="A406" s="41" t="s">
+      <c r="A406" s="69" t="s">
         <v>405</v>
       </c>
       <c r="B406">
@@ -5883,7 +5939,7 @@
       </c>
     </row>
     <row r="407">
-      <c r="A407" s="41" t="s">
+      <c r="A407" s="69" t="s">
         <v>406</v>
       </c>
       <c r="B407">
@@ -5894,7 +5950,7 @@
       </c>
     </row>
     <row r="408">
-      <c r="A408" s="41" t="s">
+      <c r="A408" s="69" t="s">
         <v>407</v>
       </c>
       <c r="B408">
@@ -5905,7 +5961,7 @@
       </c>
     </row>
     <row r="409">
-      <c r="A409" s="41" t="s">
+      <c r="A409" s="69" t="s">
         <v>408</v>
       </c>
       <c r="B409">
@@ -5916,7 +5972,7 @@
       </c>
     </row>
     <row r="410">
-      <c r="A410" s="41" t="s">
+      <c r="A410" s="69" t="s">
         <v>409</v>
       </c>
       <c r="B410">
@@ -5927,7 +5983,7 @@
       </c>
     </row>
     <row r="411">
-      <c r="A411" s="41" t="s">
+      <c r="A411" s="69" t="s">
         <v>410</v>
       </c>
       <c r="B411">
@@ -5938,7 +5994,7 @@
       </c>
     </row>
     <row r="412">
-      <c r="A412" s="41" t="s">
+      <c r="A412" s="69" t="s">
         <v>411</v>
       </c>
       <c r="B412">
@@ -5949,7 +6005,7 @@
       </c>
     </row>
     <row r="413">
-      <c r="A413" s="41" t="s">
+      <c r="A413" s="69" t="s">
         <v>412</v>
       </c>
       <c r="B413">
@@ -5960,7 +6016,7 @@
       </c>
     </row>
     <row r="414">
-      <c r="A414" s="41" t="s">
+      <c r="A414" s="69" t="s">
         <v>413</v>
       </c>
       <c r="B414">
@@ -5971,7 +6027,7 @@
       </c>
     </row>
     <row r="415">
-      <c r="A415" s="41" t="s">
+      <c r="A415" s="69" t="s">
         <v>414</v>
       </c>
       <c r="B415">
@@ -5982,7 +6038,7 @@
       </c>
     </row>
     <row r="416">
-      <c r="A416" s="41" t="s">
+      <c r="A416" s="69" t="s">
         <v>415</v>
       </c>
       <c r="B416">
@@ -5993,7 +6049,7 @@
       </c>
     </row>
     <row r="417">
-      <c r="A417" s="41" t="s">
+      <c r="A417" s="69" t="s">
         <v>416</v>
       </c>
       <c r="B417">
@@ -6004,7 +6060,7 @@
       </c>
     </row>
     <row r="418">
-      <c r="A418" s="41" t="s">
+      <c r="A418" s="69" t="s">
         <v>417</v>
       </c>
       <c r="B418">
@@ -6015,7 +6071,7 @@
       </c>
     </row>
     <row r="419">
-      <c r="A419" s="41" t="s">
+      <c r="A419" s="69" t="s">
         <v>418</v>
       </c>
       <c r="B419">
@@ -6026,7 +6082,7 @@
       </c>
     </row>
     <row r="420">
-      <c r="A420" s="41" t="s">
+      <c r="A420" s="69" t="s">
         <v>419</v>
       </c>
       <c r="B420">

</xml_diff>